<commit_message>
t5b - pequenas correções, falta incertezas
</commit_message>
<xml_diff>
--- a/T5B - elástico.xlsx
+++ b/T5B - elástico.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nunop\OneDrive\Documentos\GitHub\LABSFISICAI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D54AC25-2478-4807-B573-A90B9E503326}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59C185E1-21DB-4084-8279-7DF83090B01E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9CE87473-03DA-42DD-9F86-026CAF99A140}"/>
   </bookViews>
@@ -278,7 +278,7 @@
   <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.000"/>
-    <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -428,7 +428,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -468,13 +468,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -492,37 +519,16 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -577,20 +583,16 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
+              <a:rPr lang="pt-PT"/>
+              <a:t>F(</a:t>
+            </a:r>
+            <a:r>
               <a:rPr lang="el-GR"/>
               <a:t>Δ</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>L(</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="pt-PT"/>
-              <a:t>m</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>) - Carga</a:t>
+              <a:t>L) - Carga</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -715,7 +717,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Carga e Descarga'!$F$3:$F$15</c:f>
+              <c:f>'Carga e Descarga'!$F$4:$F$16</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="13"/>
@@ -763,7 +765,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Carga e Descarga'!$B$3:$B$15</c:f>
+              <c:f>'Carga e Descarga'!$B$4:$B$16</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="13"/>
@@ -3178,7 +3180,7 @@
             <c:spPr>
               <a:ln w="19050" cap="rnd">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:schemeClr val="accent2"/>
                 </a:solidFill>
                 <a:prstDash val="sysDot"/>
               </a:ln>
@@ -3221,7 +3223,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Carga e Descarga'!$D$3:$D$15</c:f>
+              <c:f>'Carga e Descarga'!$D$4:$D$16</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="13"/>
@@ -3269,7 +3271,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Carga e Descarga'!$B$3:$B$15</c:f>
+              <c:f>'Carga e Descarga'!$B$4:$B$16</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="13"/>
@@ -3779,7 +3781,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Carga e Descarga'!$D$3:$D$15</c:f>
+              <c:f>'Carga e Descarga'!$D$4:$D$16</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="13"/>
@@ -3827,7 +3829,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Carga e Descarga'!$Y$3:$Y$19</c:f>
+              <c:f>'Carga e Descarga'!$Y$4:$Y$20</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="17"/>
@@ -4300,7 +4302,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Carga e Descarga'!$F$3:$F$15</c:f>
+              <c:f>'Carga e Descarga'!$F$4:$F$16</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="13"/>
@@ -4348,7 +4350,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Carga e Descarga'!$AA$3:$AA$15</c:f>
+              <c:f>'Carga e Descarga'!$AA$4:$AA$16</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="13"/>
@@ -4740,7 +4742,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Carga e Descarga: </a:t>
+              <a:t>Carga e Descarga: F(</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="el-GR" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
@@ -4752,19 +4754,7 @@
               <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
                 <a:effectLst/>
               </a:rPr>
-              <a:t>L(</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="pt-PT" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:effectLst/>
-              </a:rPr>
-              <a:t>m</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:effectLst/>
-              </a:rPr>
-              <a:t>)</a:t>
+              <a:t>L)</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -4807,9 +4797,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.16434737315354525"/>
-          <c:y val="0.17378178468299524"/>
+          <c:y val="0.13784818905791824"/>
           <c:w val="0.78610886123337231"/>
-          <c:h val="0.64823624113790057"/>
+          <c:h val="0.68416959303627189"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -4874,8 +4864,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="5.1786670188721545E-2"/>
-                  <c:y val="-4.8997466463944962E-2"/>
+                  <c:x val="5.6389747716151149E-2"/>
+                  <c:y val="-3.9031268800060546E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -4910,7 +4900,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Carga e Descarga'!$D$3:$D$15</c:f>
+              <c:f>'Carga e Descarga'!$D$4:$D$16</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="13"/>
@@ -4958,7 +4948,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Carga e Descarga'!$B$3:$B$15</c:f>
+              <c:f>'Carga e Descarga'!$B$4:$B$16</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="13"/>
@@ -5056,8 +5046,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="4.6702796884730842E-2"/>
-                  <c:y val="0.33922089945260775"/>
+                  <c:x val="3.4644095665825575E-2"/>
+                  <c:y val="0.34725305584429228"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -5092,7 +5082,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Carga e Descarga'!$F$3:$F$15</c:f>
+              <c:f>'Carga e Descarga'!$F$4:$F$16</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="13"/>
@@ -5140,7 +5130,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Carga e Descarga'!$B$3:$B$15</c:f>
+              <c:f>'Carga e Descarga'!$B$4:$B$16</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="13"/>
@@ -5456,6 +5446,10 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="tr"/>
+      <c:legendEntry>
+        <c:idx val="2"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
       <c:layout>
         <c:manualLayout>
           <c:xMode val="edge"/>
@@ -5679,7 +5673,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Carga e Descarga'!$E$31:$E$43</c:f>
+              <c:f>'Carga e Descarga'!$E$32:$E$44</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="13"/>
@@ -5727,7 +5721,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Carga e Descarga'!$G$31:$G$43</c:f>
+              <c:f>'Carga e Descarga'!$G$32:$G$44</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="13"/>
@@ -5810,7 +5804,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Carga e Descarga'!$F$31:$F$43</c:f>
+              <c:f>'Carga e Descarga'!$F$32:$F$44</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="13"/>
@@ -5858,7 +5852,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Carga e Descarga'!$G$31:$G$43</c:f>
+              <c:f>'Carga e Descarga'!$G$32:$G$44</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="13"/>
@@ -14724,13 +14718,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>188767</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>65659</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>181840</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>3463</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -14768,7 +14762,7 @@
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>59378</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>12273</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -14800,13 +14794,13 @@
     <xdr:from>
       <xdr:col>18</xdr:col>
       <xdr:colOff>191364</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>125928</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
       <xdr:colOff>416502</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>103662</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -14842,7 +14836,7 @@
     <xdr:to>
       <xdr:col>25</xdr:col>
       <xdr:colOff>362692</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>162792</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -14874,13 +14868,13 @@
     <xdr:from>
       <xdr:col>18</xdr:col>
       <xdr:colOff>123746</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>47042</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
       <xdr:colOff>330574</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>51780</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -14910,13 +14904,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>143977</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>69520</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>51955</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>90054</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -15471,10 +15465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{011F8627-D91A-4233-8512-CFE2F65682AE}">
-  <dimension ref="A1:AE44"/>
+  <dimension ref="A1:AE45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+      <selection activeCell="F3" sqref="C3:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15491,25 +15485,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="X1" s="20" t="s">
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="X1" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="Y1" s="20"/>
-      <c r="Z1" s="20" t="s">
+      <c r="Y1" s="29"/>
+      <c r="Z1" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="AA1" s="20"/>
+      <c r="AA1" s="29"/>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
@@ -15553,123 +15547,90 @@
       </c>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A3" s="17">
-        <v>1.0240000000000001E-2</v>
-      </c>
-      <c r="B3" s="17">
-        <f>A3*9.81</f>
-        <v>0.10045440000000001</v>
-      </c>
-      <c r="C3" s="17">
-        <v>0.41299999999999998</v>
-      </c>
-      <c r="D3" s="17">
-        <f t="shared" ref="D3:D15" si="0">C3-$G$17</f>
-        <v>0</v>
-      </c>
-      <c r="E3" s="17">
-        <v>0.41699999999999998</v>
-      </c>
-      <c r="F3" s="17">
-        <f t="shared" ref="F3:F15" si="1">E3-$G$17</f>
-        <v>4.0000000000000036E-3</v>
-      </c>
-      <c r="G3" s="4">
-        <v>3.28E-4</v>
-      </c>
-      <c r="H3" s="4">
-        <v>4.2700000000000002E-4</v>
-      </c>
-      <c r="I3" s="4">
-        <f>G3*H3</f>
-        <v>1.4005600000000002E-7</v>
-      </c>
-      <c r="X3" s="18">
-        <f>$A$19*D3^3+$B$19*D3^2+$C$19*D3+$D$19</f>
-        <v>0.11543688973114569</v>
-      </c>
-      <c r="Y3" s="18">
-        <f>B3-X3</f>
-        <v>-1.4982489731145673E-2</v>
-      </c>
-      <c r="Z3" s="18">
-        <f>$A$23*(F3^3)+$B$23*(F3^2)+$C$23*F3+$D$23</f>
-        <v>0.1138750385595301</v>
-      </c>
-      <c r="AA3" s="18">
-        <f>B3-Z3</f>
-        <v>-1.3420638559530088E-2</v>
-      </c>
+      <c r="A3" s="21"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="X3" s="20"/>
+      <c r="Y3" s="20"/>
+      <c r="Z3" s="20"/>
+      <c r="AA3" s="20"/>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A4" s="17">
-        <v>2.0250000000000001E-2</v>
+        <v>1.0240000000000001E-2</v>
       </c>
       <c r="B4" s="17">
-        <f t="shared" ref="B4:B15" si="2">A4*9.81</f>
-        <v>0.19865250000000001</v>
+        <f>A4*9.81</f>
+        <v>0.10045440000000001</v>
       </c>
       <c r="C4" s="17">
-        <v>0.41899999999999998</v>
+        <v>0.41299999999999998</v>
       </c>
       <c r="D4" s="17">
-        <f t="shared" si="0"/>
-        <v>6.0000000000000053E-3</v>
+        <f t="shared" ref="D4:D16" si="0">C4-$G$18</f>
+        <v>0</v>
       </c>
       <c r="E4" s="17">
-        <v>0.42399999999999999</v>
+        <v>0.41699999999999998</v>
       </c>
       <c r="F4" s="17">
-        <f t="shared" si="1"/>
-        <v>1.100000000000001E-2</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>4</v>
+        <f t="shared" ref="F4:F16" si="1">E4-$G$18</f>
+        <v>4.0000000000000036E-3</v>
+      </c>
+      <c r="G4" s="4">
+        <v>3.28E-4</v>
+      </c>
+      <c r="H4" s="4">
+        <v>4.2700000000000002E-4</v>
+      </c>
+      <c r="I4" s="4">
+        <f>G4*H4</f>
+        <v>1.4005600000000002E-7</v>
       </c>
       <c r="X4" s="18">
-        <f>$A$19*D4^3+$B$19*D4^2+$C$19*D4+$D$19</f>
-        <v>0.19364495040707835</v>
+        <f t="shared" ref="X4:X16" si="2">$A$20*D4^3+$B$20*D4^2+$C$20*D4+$D$20</f>
+        <v>0.11543688973114569</v>
       </c>
       <c r="Y4" s="18">
-        <f t="shared" ref="Y4:Y15" si="3">B4-X4</f>
-        <v>5.0075495929216562E-3</v>
+        <f>B4-X4</f>
+        <v>-1.4982489731145673E-2</v>
       </c>
       <c r="Z4" s="18">
-        <f>$A$23*(F4^3)+$B$23*(F4^2)+$C$23*F4+$D$23</f>
-        <v>0.19434772374568215</v>
+        <f t="shared" ref="Z4:Z16" si="3">$A$24*(F4^3)+$B$24*(F4^2)+$C$24*F4+$D$24</f>
+        <v>0.1138750385595301</v>
       </c>
       <c r="AA4" s="18">
-        <f t="shared" ref="AA4:AA15" si="4">B4-Z4</f>
-        <v>4.3047762543178547E-3</v>
+        <f>B4-Z4</f>
+        <v>-1.3420638559530088E-2</v>
       </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A5" s="17">
-        <v>3.0339999999999999E-2</v>
+        <v>2.0250000000000001E-2</v>
       </c>
       <c r="B5" s="17">
-        <f t="shared" si="2"/>
-        <v>0.29763539999999999</v>
+        <f t="shared" ref="B5:B16" si="4">A5*9.81</f>
+        <v>0.19865250000000001</v>
       </c>
       <c r="C5" s="17">
-        <v>0.42699999999999999</v>
+        <v>0.41899999999999998</v>
       </c>
       <c r="D5" s="17">
         <f t="shared" si="0"/>
-        <v>1.4000000000000012E-2</v>
+        <v>6.0000000000000053E-3</v>
       </c>
       <c r="E5" s="17">
-        <v>0.433</v>
+        <v>0.42399999999999999</v>
       </c>
       <c r="F5" s="17">
         <f t="shared" si="1"/>
-        <v>2.0000000000000018E-2</v>
+        <v>1.100000000000001E-2</v>
       </c>
       <c r="G5" s="5" t="s">
         <v>4</v>
@@ -15681,43 +15642,43 @@
         <v>4</v>
       </c>
       <c r="X5" s="18">
-        <f>$A$19*D5^3+$B$19*D5^2+$C$19*D5+$D$19</f>
-        <v>0.28999942529810896</v>
+        <f t="shared" si="2"/>
+        <v>0.19364495040707835</v>
       </c>
       <c r="Y5" s="18">
+        <f t="shared" ref="Y5:Y16" si="5">B5-X5</f>
+        <v>5.0075495929216562E-3</v>
+      </c>
+      <c r="Z5" s="18">
         <f t="shared" si="3"/>
-        <v>7.6359747018910351E-3</v>
-      </c>
-      <c r="Z5" s="18">
-        <f>$A$23*(F5^3)+$B$23*(F5^2)+$C$23*F5+$D$23</f>
-        <v>0.28942658841201363</v>
+        <v>0.19434772374568215</v>
       </c>
       <c r="AA5" s="18">
-        <f t="shared" si="4"/>
-        <v>8.2088115879863643E-3</v>
+        <f t="shared" ref="AA5:AA16" si="6">B5-Z5</f>
+        <v>4.3047762543178547E-3</v>
       </c>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A6" s="17">
-        <v>4.0489999999999998E-2</v>
+        <v>3.0339999999999999E-2</v>
       </c>
       <c r="B6" s="17">
-        <f t="shared" si="2"/>
-        <v>0.39720690000000003</v>
+        <f t="shared" si="4"/>
+        <v>0.29763539999999999</v>
       </c>
       <c r="C6" s="17">
-        <v>0.436</v>
+        <v>0.42699999999999999</v>
       </c>
       <c r="D6" s="17">
         <f t="shared" si="0"/>
-        <v>2.300000000000002E-2</v>
+        <v>1.4000000000000012E-2</v>
       </c>
       <c r="E6" s="17">
-        <v>0.443</v>
+        <v>0.433</v>
       </c>
       <c r="F6" s="17">
         <f t="shared" si="1"/>
-        <v>3.0000000000000027E-2</v>
+        <v>2.0000000000000018E-2</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>4</v>
@@ -15729,43 +15690,43 @@
         <v>4</v>
       </c>
       <c r="X6" s="18">
-        <f>$A$19*D6^3+$B$19*D6^2+$C$19*D6+$D$19</f>
-        <v>0.38830599108672942</v>
+        <f t="shared" si="2"/>
+        <v>0.28999942529810896</v>
       </c>
       <c r="Y6" s="18">
+        <f t="shared" si="5"/>
+        <v>7.6359747018910351E-3</v>
+      </c>
+      <c r="Z6" s="18">
         <f t="shared" si="3"/>
-        <v>8.900908913270611E-3</v>
-      </c>
-      <c r="Z6" s="18">
-        <f>$A$23*(F6^3)+$B$23*(F6^2)+$C$23*F6+$D$23</f>
-        <v>0.38494431336259582</v>
+        <v>0.28942658841201363</v>
       </c>
       <c r="AA6" s="18">
-        <f t="shared" si="4"/>
-        <v>1.2262586637404205E-2</v>
+        <f t="shared" si="6"/>
+        <v>8.2088115879863643E-3</v>
       </c>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A7" s="17">
-        <v>5.0560000000000001E-2</v>
+        <v>4.0489999999999998E-2</v>
       </c>
       <c r="B7" s="17">
-        <f t="shared" si="2"/>
-        <v>0.49599360000000003</v>
+        <f t="shared" si="4"/>
+        <v>0.39720690000000003</v>
       </c>
       <c r="C7" s="17">
-        <v>0.44700000000000001</v>
+        <v>0.436</v>
       </c>
       <c r="D7" s="17">
         <f t="shared" si="0"/>
-        <v>3.400000000000003E-2</v>
+        <v>2.300000000000002E-2</v>
       </c>
       <c r="E7" s="17">
-        <v>0.45600000000000002</v>
+        <v>0.443</v>
       </c>
       <c r="F7" s="17">
         <f t="shared" si="1"/>
-        <v>4.3000000000000038E-2</v>
+        <v>3.0000000000000027E-2</v>
       </c>
       <c r="G7" s="5" t="s">
         <v>4</v>
@@ -15777,43 +15738,43 @@
         <v>4</v>
       </c>
       <c r="X7" s="18">
-        <f>$A$19*D7^3+$B$19*D7^2+$C$19*D7+$D$19</f>
-        <v>0.49522653182815812</v>
+        <f t="shared" si="2"/>
+        <v>0.38830599108672942</v>
       </c>
       <c r="Y7" s="18">
+        <f t="shared" si="5"/>
+        <v>8.900908913270611E-3</v>
+      </c>
+      <c r="Z7" s="18">
         <f t="shared" si="3"/>
-        <v>7.6706817184191145E-4</v>
-      </c>
-      <c r="Z7" s="18">
-        <f>$A$23*(F7^3)+$B$23*(F7^2)+$C$23*F7+$D$23</f>
-        <v>0.4950025994997459</v>
+        <v>0.38494431336259582</v>
       </c>
       <c r="AA7" s="18">
-        <f t="shared" si="4"/>
-        <v>9.9100050025413555E-4</v>
+        <f t="shared" si="6"/>
+        <v>1.2262586637404205E-2</v>
       </c>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A8" s="17">
-        <v>6.0609999999999997E-2</v>
+        <v>5.0560000000000001E-2</v>
       </c>
       <c r="B8" s="17">
-        <f t="shared" si="2"/>
-        <v>0.59458409999999995</v>
+        <f t="shared" si="4"/>
+        <v>0.49599360000000003</v>
       </c>
       <c r="C8" s="17">
-        <v>0.45800000000000002</v>
+        <v>0.44700000000000001</v>
       </c>
       <c r="D8" s="17">
         <f t="shared" si="0"/>
-        <v>4.500000000000004E-2</v>
+        <v>3.400000000000003E-2</v>
       </c>
       <c r="E8" s="17">
-        <v>0.47</v>
+        <v>0.45600000000000002</v>
       </c>
       <c r="F8" s="17">
         <f t="shared" si="1"/>
-        <v>5.6999999999999995E-2</v>
+        <v>4.3000000000000038E-2</v>
       </c>
       <c r="G8" s="5" t="s">
         <v>4</v>
@@ -15825,43 +15786,43 @@
         <v>4</v>
       </c>
       <c r="X8" s="18">
-        <f>$A$19*D8^3+$B$19*D8^2+$C$19*D8+$D$19</f>
-        <v>0.58915051373090188</v>
+        <f t="shared" si="2"/>
+        <v>0.49522653182815812</v>
       </c>
       <c r="Y8" s="18">
+        <f t="shared" si="5"/>
+        <v>7.6706817184191145E-4</v>
+      </c>
+      <c r="Z8" s="18">
         <f t="shared" si="3"/>
-        <v>5.4335862690980674E-3</v>
-      </c>
-      <c r="Z8" s="18">
-        <f>$A$23*(F8^3)+$B$23*(F8^2)+$C$23*F8+$D$23</f>
-        <v>0.59834250902307207</v>
+        <v>0.4950025994997459</v>
       </c>
       <c r="AA8" s="18">
-        <f t="shared" si="4"/>
-        <v>-3.7584090230721179E-3</v>
+        <f t="shared" si="6"/>
+        <v>9.9100050025413555E-4</v>
       </c>
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A9" s="17">
-        <v>7.0650000000000004E-2</v>
+        <v>6.0609999999999997E-2</v>
       </c>
       <c r="B9" s="17">
-        <f t="shared" si="2"/>
-        <v>0.6930765000000001</v>
+        <f t="shared" si="4"/>
+        <v>0.59458409999999995</v>
       </c>
       <c r="C9" s="17">
-        <v>0.47299999999999998</v>
+        <v>0.45800000000000002</v>
       </c>
       <c r="D9" s="17">
         <f t="shared" si="0"/>
-        <v>0.06</v>
+        <v>4.500000000000004E-2</v>
       </c>
       <c r="E9" s="17">
-        <v>0.48699999999999999</v>
+        <v>0.47</v>
       </c>
       <c r="F9" s="17">
         <f t="shared" si="1"/>
-        <v>7.400000000000001E-2</v>
+        <v>5.6999999999999995E-2</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>4</v>
@@ -15873,43 +15834,43 @@
         <v>4</v>
       </c>
       <c r="X9" s="18">
-        <f>$A$19*D9^3+$B$19*D9^2+$C$19*D9+$D$19</f>
-        <v>0.69928167827754861</v>
+        <f t="shared" si="2"/>
+        <v>0.58915051373090188</v>
       </c>
       <c r="Y9" s="18">
+        <f t="shared" si="5"/>
+        <v>5.4335862690980674E-3</v>
+      </c>
+      <c r="Z9" s="18">
         <f t="shared" si="3"/>
-        <v>-6.2051782775485176E-3</v>
-      </c>
-      <c r="Z9" s="18">
-        <f>$A$23*(F9^3)+$B$23*(F9^2)+$C$23*F9+$D$23</f>
-        <v>0.7070664921675025</v>
+        <v>0.59834250902307207</v>
       </c>
       <c r="AA9" s="18">
-        <f t="shared" si="4"/>
-        <v>-1.3989992167502407E-2</v>
+        <f t="shared" si="6"/>
+        <v>-3.7584090230721179E-3</v>
       </c>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A10" s="17">
-        <v>8.0750000000000002E-2</v>
+        <v>7.0650000000000004E-2</v>
       </c>
       <c r="B10" s="17">
-        <f t="shared" si="2"/>
-        <v>0.79215750000000007</v>
+        <f t="shared" si="4"/>
+        <v>0.6930765000000001</v>
       </c>
       <c r="C10" s="17">
-        <v>0.49</v>
+        <v>0.47299999999999998</v>
       </c>
       <c r="D10" s="17">
         <f t="shared" si="0"/>
-        <v>7.7000000000000013E-2</v>
+        <v>0.06</v>
       </c>
       <c r="E10" s="17">
-        <v>0.504</v>
+        <v>0.48699999999999999</v>
       </c>
       <c r="F10" s="17">
         <f t="shared" si="1"/>
-        <v>9.1000000000000025E-2</v>
+        <v>7.400000000000001E-2</v>
       </c>
       <c r="G10" s="5" t="s">
         <v>4</v>
@@ -15921,43 +15882,43 @@
         <v>4</v>
       </c>
       <c r="X10" s="18">
-        <f>$A$19*D10^3+$B$19*D10^2+$C$19*D10+$D$19</f>
-        <v>0.80392300115051696</v>
+        <f t="shared" si="2"/>
+        <v>0.69928167827754861</v>
       </c>
       <c r="Y10" s="18">
+        <f t="shared" si="5"/>
+        <v>-6.2051782775485176E-3</v>
+      </c>
+      <c r="Z10" s="18">
         <f t="shared" si="3"/>
-        <v>-1.1765501150516888E-2</v>
-      </c>
-      <c r="Z10" s="18">
-        <f>$A$23*(F10^3)+$B$23*(F10^2)+$C$23*F10+$D$23</f>
-        <v>0.80268431952747932</v>
+        <v>0.7070664921675025</v>
       </c>
       <c r="AA10" s="18">
-        <f t="shared" si="4"/>
-        <v>-1.0526819527479248E-2</v>
+        <f t="shared" si="6"/>
+        <v>-1.3989992167502407E-2</v>
       </c>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A11" s="17">
-        <v>9.0929999999999997E-2</v>
+        <v>8.0750000000000002E-2</v>
       </c>
       <c r="B11" s="17">
-        <f t="shared" si="2"/>
-        <v>0.89202329999999996</v>
+        <f t="shared" si="4"/>
+        <v>0.79215750000000007</v>
       </c>
       <c r="C11" s="17">
-        <v>0.50700000000000001</v>
+        <v>0.49</v>
       </c>
       <c r="D11" s="17">
         <f t="shared" si="0"/>
-        <v>9.4000000000000028E-2</v>
+        <v>7.7000000000000013E-2</v>
       </c>
       <c r="E11" s="17">
-        <v>0.51900000000000002</v>
+        <v>0.504</v>
       </c>
       <c r="F11" s="17">
         <f t="shared" si="1"/>
-        <v>0.10600000000000004</v>
+        <v>9.1000000000000025E-2</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>4</v>
@@ -15969,43 +15930,43 @@
         <v>4</v>
       </c>
       <c r="X11" s="18">
-        <f>$A$19*D11^3+$B$19*D11^2+$C$19*D11+$D$19</f>
-        <v>0.89301343109781373</v>
+        <f t="shared" si="2"/>
+        <v>0.80392300115051696</v>
       </c>
       <c r="Y11" s="18">
+        <f t="shared" si="5"/>
+        <v>-1.1765501150516888E-2</v>
+      </c>
+      <c r="Z11" s="18">
         <f t="shared" si="3"/>
-        <v>-9.901310978137623E-4</v>
-      </c>
-      <c r="Z11" s="18">
-        <f>$A$23*(F11^3)+$B$23*(F11^2)+$C$23*F11+$D$23</f>
-        <v>0.88064171190349305</v>
+        <v>0.80268431952747932</v>
       </c>
       <c r="AA11" s="18">
-        <f t="shared" si="4"/>
-        <v>1.1381588096506912E-2</v>
+        <f t="shared" si="6"/>
+        <v>-1.0526819527479248E-2</v>
       </c>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A12" s="17">
-        <v>0.10097</v>
+        <v>9.0929999999999997E-2</v>
       </c>
       <c r="B12" s="17">
-        <f t="shared" si="2"/>
-        <v>0.99051570000000011</v>
+        <f t="shared" si="4"/>
+        <v>0.89202329999999996</v>
       </c>
       <c r="C12" s="17">
-        <v>0.52900000000000003</v>
+        <v>0.50700000000000001</v>
       </c>
       <c r="D12" s="17">
         <f t="shared" si="0"/>
-        <v>0.11600000000000005</v>
+        <v>9.4000000000000028E-2</v>
       </c>
       <c r="E12" s="17">
-        <v>0.53900000000000003</v>
+        <v>0.51900000000000002</v>
       </c>
       <c r="F12" s="17">
         <f t="shared" si="1"/>
-        <v>0.12600000000000006</v>
+        <v>0.10600000000000004</v>
       </c>
       <c r="G12" s="5" t="s">
         <v>4</v>
@@ -16017,43 +15978,43 @@
         <v>4</v>
       </c>
       <c r="X12" s="18">
-        <f>$A$19*D12^3+$B$19*D12^2+$C$19*D12+$D$19</f>
-        <v>0.99520484458816205</v>
+        <f t="shared" si="2"/>
+        <v>0.89301343109781373</v>
       </c>
       <c r="Y12" s="18">
+        <f t="shared" si="5"/>
+        <v>-9.901310978137623E-4</v>
+      </c>
+      <c r="Z12" s="18">
         <f t="shared" si="3"/>
-        <v>-4.689144588161942E-3</v>
-      </c>
-      <c r="Z12" s="18">
-        <f>$A$23*(F12^3)+$B$23*(F12^2)+$C$23*F12+$D$23</f>
-        <v>0.98215719604090768</v>
+        <v>0.88064171190349305</v>
       </c>
       <c r="AA12" s="18">
-        <f t="shared" si="4"/>
-        <v>8.3585039590924337E-3</v>
+        <f t="shared" si="6"/>
+        <v>1.1381588096506912E-2</v>
       </c>
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A13" s="17">
-        <v>0.11103</v>
+        <v>0.10097</v>
       </c>
       <c r="B13" s="17">
-        <f t="shared" si="2"/>
-        <v>1.0892043</v>
+        <f t="shared" si="4"/>
+        <v>0.99051570000000011</v>
       </c>
       <c r="C13" s="17">
-        <v>0.54700000000000004</v>
+        <v>0.52900000000000003</v>
       </c>
       <c r="D13" s="17">
         <f t="shared" si="0"/>
-        <v>0.13400000000000006</v>
+        <v>0.11600000000000005</v>
       </c>
       <c r="E13" s="17">
-        <v>0.55900000000000005</v>
+        <v>0.53900000000000003</v>
       </c>
       <c r="F13" s="17">
         <f t="shared" si="1"/>
-        <v>0.14600000000000007</v>
+        <v>0.12600000000000006</v>
       </c>
       <c r="G13" s="5" t="s">
         <v>4</v>
@@ -16065,43 +16026,43 @@
         <v>4</v>
       </c>
       <c r="X13" s="18">
-        <f>$A$19*D13^3+$B$19*D13^2+$C$19*D13+$D$19</f>
-        <v>1.0763474259512305</v>
+        <f t="shared" si="2"/>
+        <v>0.99520484458816205</v>
       </c>
       <c r="Y13" s="18">
+        <f t="shared" si="5"/>
+        <v>-4.689144588161942E-3</v>
+      </c>
+      <c r="Z13" s="18">
         <f t="shared" si="3"/>
-        <v>1.2856874048769562E-2</v>
-      </c>
-      <c r="Z13" s="18">
-        <f>$A$23*(F13^3)+$B$23*(F13^2)+$C$23*F13+$D$23</f>
-        <v>1.089265503901349</v>
+        <v>0.98215719604090768</v>
       </c>
       <c r="AA13" s="18">
-        <f t="shared" si="4"/>
-        <v>-6.1203901349005108E-5</v>
+        <f t="shared" si="6"/>
+        <v>8.3585039590924337E-3</v>
       </c>
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A14" s="17">
-        <v>0.12107999999999999</v>
+        <v>0.11103</v>
       </c>
       <c r="B14" s="17">
-        <f t="shared" si="2"/>
-        <v>1.1877948</v>
+        <f t="shared" si="4"/>
+        <v>1.0892043</v>
       </c>
       <c r="C14" s="17">
-        <v>0.56899999999999995</v>
+        <v>0.54700000000000004</v>
       </c>
       <c r="D14" s="17">
         <f t="shared" si="0"/>
-        <v>0.15599999999999997</v>
+        <v>0.13400000000000006</v>
       </c>
       <c r="E14" s="17">
-        <v>0.57599999999999996</v>
+        <v>0.55900000000000005</v>
       </c>
       <c r="F14" s="17">
         <f t="shared" si="1"/>
-        <v>0.16299999999999998</v>
+        <v>0.14600000000000007</v>
       </c>
       <c r="G14" s="5" t="s">
         <v>4</v>
@@ -16113,725 +16074,773 @@
         <v>4</v>
       </c>
       <c r="X14" s="18">
-        <f>$A$19*D14^3+$B$19*D14^2+$C$19*D14+$D$19</f>
-        <v>1.1838395452102002</v>
+        <f t="shared" si="2"/>
+        <v>1.0763474259512305</v>
       </c>
       <c r="Y14" s="18">
+        <f t="shared" si="5"/>
+        <v>1.2856874048769562E-2</v>
+      </c>
+      <c r="Z14" s="18">
         <f t="shared" si="3"/>
-        <v>3.9552547897998558E-3</v>
-      </c>
-      <c r="Z14" s="18">
-        <f>$A$23*(F14^3)+$B$23*(F14^2)+$C$23*F14+$D$23</f>
-        <v>1.1915229778502316</v>
+        <v>1.089265503901349</v>
       </c>
       <c r="AA14" s="18">
-        <f t="shared" si="4"/>
-        <v>-3.7281778502316065E-3</v>
+        <f t="shared" si="6"/>
+        <v>-6.1203901349005108E-5</v>
       </c>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A15" s="17">
-        <v>0.13125999999999999</v>
+        <v>0.12107999999999999</v>
       </c>
       <c r="B15" s="17">
-        <f t="shared" si="2"/>
-        <v>1.2876605999999999</v>
+        <f t="shared" si="4"/>
+        <v>1.1877948</v>
       </c>
       <c r="C15" s="17">
-        <v>0.58799999999999997</v>
+        <v>0.56899999999999995</v>
       </c>
       <c r="D15" s="17">
         <f t="shared" si="0"/>
-        <v>0.17499999999999999</v>
+        <v>0.15599999999999997</v>
       </c>
       <c r="E15" s="17">
-        <v>0.59</v>
+        <v>0.57599999999999996</v>
       </c>
       <c r="F15" s="17">
         <f t="shared" si="1"/>
+        <v>0.16299999999999998</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="X15" s="18">
+        <f t="shared" si="2"/>
+        <v>1.1838395452102002</v>
+      </c>
+      <c r="Y15" s="18">
+        <f t="shared" si="5"/>
+        <v>3.9552547897998558E-3</v>
+      </c>
+      <c r="Z15" s="18">
+        <f t="shared" si="3"/>
+        <v>1.1915229778502316</v>
+      </c>
+      <c r="AA15" s="18">
+        <f t="shared" si="6"/>
+        <v>-3.7281778502316065E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A16" s="17">
+        <v>0.13125999999999999</v>
+      </c>
+      <c r="B16" s="17">
+        <f t="shared" si="4"/>
+        <v>1.2876605999999999</v>
+      </c>
+      <c r="C16" s="17">
+        <v>0.58799999999999997</v>
+      </c>
+      <c r="D16" s="17">
+        <f t="shared" si="0"/>
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="E16" s="17">
+        <v>0.59</v>
+      </c>
+      <c r="F16" s="17">
+        <f t="shared" si="1"/>
         <v>0.17699999999999999</v>
       </c>
-      <c r="G15" s="4">
+      <c r="G16" s="4">
         <v>2.24E-4</v>
       </c>
-      <c r="H15" s="4">
+      <c r="H16" s="4">
         <v>4.1300000000000001E-4</v>
       </c>
-      <c r="I15" s="4">
-        <f>G15*H15</f>
+      <c r="I16" s="4">
+        <f>G16*H16</f>
         <v>9.2512000000000001E-8</v>
       </c>
-      <c r="X15" s="18">
-        <f>$A$19*D15^3+$B$19*D15^2+$C$19*D15+$D$19</f>
+      <c r="X16" s="18">
+        <f t="shared" si="2"/>
         <v>1.2935853716424059</v>
       </c>
-      <c r="Y15" s="18">
+      <c r="Y16" s="18">
+        <f t="shared" si="5"/>
+        <v>-5.9247716424060126E-3</v>
+      </c>
+      <c r="Z16" s="18">
         <f t="shared" si="3"/>
-        <v>-5.9247716424060126E-3</v>
-      </c>
-      <c r="Z15" s="18">
-        <f>$A$23*(F15^3)+$B$23*(F15^2)+$C$23*F15+$D$23</f>
         <v>1.287682626006394</v>
       </c>
-      <c r="AA15" s="18">
-        <f t="shared" si="4"/>
+      <c r="AA16" s="18">
+        <f t="shared" si="6"/>
         <v>-2.2026006394115782E-5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="35" t="s">
-        <v>44</v>
-      </c>
-      <c r="B17" s="35"/>
-      <c r="C17" s="35"/>
-      <c r="D17" s="35"/>
-      <c r="F17" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="G17" s="28">
-        <f>C3</f>
-        <v>0.41299999999999998</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="C18" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="D18" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="F18" s="33"/>
-      <c r="G18" s="33"/>
+      <c r="A18" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" s="34"/>
+      <c r="C18" s="34"/>
+      <c r="D18" s="34"/>
+      <c r="F18" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="G18" s="22">
+        <f>C4</f>
+        <v>0.41299999999999998</v>
+      </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19" s="4">
-        <f t="array" ref="A19:D19">LINEST(B3:B15,D3:D15^{1,2,3},TRUE,TRUE)</f>
-        <v>207.75294223761728</v>
-      </c>
-      <c r="B19" s="4">
-        <v>-74.895588697844104</v>
-      </c>
-      <c r="C19" s="4">
-        <v>13.476571205588607</v>
-      </c>
-      <c r="D19" s="4">
-        <v>0.11543688973114569</v>
-      </c>
-      <c r="F19" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>24</v>
-      </c>
+      <c r="A19" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="F19" s="27"/>
+      <c r="G19" s="27"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F20" s="4">
-        <f>D3</f>
-        <v>0</v>
-      </c>
-      <c r="G20" s="4">
-        <f>I3</f>
-        <v>1.4005600000000002E-7</v>
+      <c r="A20" s="4">
+        <f t="array" ref="A20:D20">LINEST(B4:B16,D4:D16^{1,2,3},TRUE,TRUE)</f>
+        <v>207.75294223761728</v>
+      </c>
+      <c r="B20" s="4">
+        <v>-74.895588697844104</v>
+      </c>
+      <c r="C20" s="4">
+        <v>13.476571205588607</v>
+      </c>
+      <c r="D20" s="4">
+        <v>0.11543688973114569</v>
+      </c>
+      <c r="F20" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" s="35" t="s">
-        <v>45</v>
-      </c>
-      <c r="B21" s="35"/>
-      <c r="C21" s="35"/>
-      <c r="D21" s="35"/>
       <c r="F21" s="4">
-        <f>D15</f>
-        <v>0.17499999999999999</v>
+        <f>D4</f>
+        <v>0</v>
       </c>
       <c r="G21" s="4">
-        <f>I15</f>
-        <v>9.2512000000000001E-8</v>
+        <f>I4</f>
+        <v>1.4005600000000002E-7</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="B22" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="C22" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="D22" s="19" t="s">
-        <v>20</v>
+      <c r="A22" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" s="34"/>
+      <c r="C22" s="34"/>
+      <c r="D22" s="34"/>
+      <c r="F22" s="4">
+        <f>D16</f>
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="G22" s="4">
+        <f>I16</f>
+        <v>9.2512000000000001E-8</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23" s="4">
-        <f t="array" ref="A23:D23">LINEST(B3:B15,F3:F15^{1,2,3},TRUE,TRUE)</f>
+      <c r="A23" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="B23" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="D23" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" s="4">
+        <f t="array" ref="A24:D24">LINEST(B4:B16,F4:F16^{1,2,3},TRUE,TRUE)</f>
         <v>190.1669209069772</v>
       </c>
-      <c r="B23" s="4">
+      <c r="B24" s="4">
         <v>-64.892066449053743</v>
       </c>
-      <c r="C23" s="4">
+      <c r="C24" s="4">
         <v>12.435058667787642</v>
       </c>
-      <c r="D23" s="4">
+      <c r="D24" s="4">
         <v>6.5160906268626306E-2</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B25" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="C25" s="21"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B26" s="4">
-        <f t="array" ref="B26:C28">LINEST(G20:G21,F20:F21,TRUE,TRUE)</f>
-        <v>-2.7168000000000022E-7</v>
-      </c>
-      <c r="C26" s="4">
-        <v>1.4005600000000002E-7</v>
-      </c>
-      <c r="D26" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="E26" s="21"/>
+      <c r="B26" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="C26" s="30"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A27" s="31" t="s">
+      <c r="A27" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" s="4">
+        <f t="array" ref="B27:C29">LINEST(G21:G22,F21:F22,TRUE,TRUE)</f>
+        <v>-2.7168000000000022E-7</v>
+      </c>
+      <c r="C27" s="4">
+        <v>1.4005600000000002E-7</v>
+      </c>
+      <c r="D27" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="E27" s="30"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="B27" s="4">
+      <c r="B28" s="4">
         <v>0</v>
-      </c>
-      <c r="C27" s="4">
-        <v>0</v>
-      </c>
-      <c r="D27" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="E27" s="21"/>
-    </row>
-    <row r="28" spans="1:8" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A28" s="31" t="s">
-        <v>43</v>
-      </c>
-      <c r="B28" s="4">
-        <v>1</v>
       </c>
       <c r="C28" s="4">
         <v>0</v>
       </c>
-      <c r="D28" s="22" t="s">
+      <c r="D28" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="E28" s="30"/>
+    </row>
+    <row r="29" spans="1:8" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A29" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="B29" s="4">
+        <v>1</v>
+      </c>
+      <c r="C29" s="4">
+        <v>0</v>
+      </c>
+      <c r="D29" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="E28" s="21"/>
+      <c r="E29" s="30"/>
     </row>
-    <row r="30" spans="1:8" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A30" s="12" t="s">
+    <row r="31" spans="1:8" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A31" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="B30" s="13" t="s">
+      <c r="B31" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C30" s="13" t="s">
+      <c r="C31" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="D30" s="13" t="s">
+      <c r="D31" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="E30" s="14" t="s">
+      <c r="E31" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="F30" s="12" t="s">
+      <c r="F31" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="G30" s="13" t="s">
+      <c r="G31" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="H30" s="13" t="s">
+      <c r="H31" s="13" t="s">
         <v>41</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A31" s="32">
-        <f>B3</f>
-        <v>0.10045440000000001</v>
-      </c>
-      <c r="B31" s="32">
-        <f>D3</f>
-        <v>0</v>
-      </c>
-      <c r="C31" s="32">
-        <f>F3</f>
-        <v>4.0000000000000036E-3</v>
-      </c>
-      <c r="D31" s="28">
-        <f>$B$26*D3+$C$26</f>
-        <v>1.4005600000000002E-7</v>
-      </c>
-      <c r="E31" s="32">
-        <f>D3/$G$17</f>
-        <v>0</v>
-      </c>
-      <c r="F31" s="17">
-        <f>F3/$G$17</f>
-        <v>9.6852300242130842E-3</v>
-      </c>
-      <c r="G31" s="28">
-        <f>A31/D31</f>
-        <v>717244.5307591249</v>
-      </c>
-      <c r="H31" s="16" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A32" s="32">
-        <f>B4</f>
-        <v>0.19865250000000001</v>
-      </c>
-      <c r="B32" s="32">
-        <f>D4</f>
-        <v>6.0000000000000053E-3</v>
-      </c>
-      <c r="C32" s="32">
-        <f>F4</f>
-        <v>1.100000000000001E-2</v>
-      </c>
-      <c r="D32" s="28">
-        <f>$B$26*D4+$C$26</f>
-        <v>1.3842592000000003E-7</v>
-      </c>
-      <c r="E32" s="32">
-        <f>D4/$G$17</f>
-        <v>1.4527845036319625E-2</v>
+      <c r="A32" s="26">
+        <f t="shared" ref="A32:A44" si="7">B4</f>
+        <v>0.10045440000000001</v>
+      </c>
+      <c r="B32" s="26">
+        <f t="shared" ref="B32:B44" si="8">D4</f>
+        <v>0</v>
+      </c>
+      <c r="C32" s="26">
+        <f t="shared" ref="C32:C44" si="9">F4</f>
+        <v>4.0000000000000036E-3</v>
+      </c>
+      <c r="D32" s="22">
+        <f t="shared" ref="D32:D44" si="10">$B$27*D4+$C$27</f>
+        <v>1.4005600000000002E-7</v>
+      </c>
+      <c r="E32" s="26">
+        <f t="shared" ref="E32:E44" si="11">D4/$G$18</f>
+        <v>0</v>
       </c>
       <c r="F32" s="17">
-        <f>F4/$G$17</f>
-        <v>2.6634382566585981E-2</v>
-      </c>
-      <c r="G32" s="28">
-        <f t="shared" ref="G32:G43" si="5">A32/D32</f>
-        <v>1435081.6667861047</v>
-      </c>
-      <c r="H32" s="28">
-        <f>G32/F32</f>
-        <v>53880793.489332788</v>
+        <f t="shared" ref="F32:F44" si="12">F4/$G$18</f>
+        <v>9.6852300242130842E-3</v>
+      </c>
+      <c r="G32" s="22">
+        <f>A32/D32</f>
+        <v>717244.5307591249</v>
+      </c>
+      <c r="H32" s="16" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="33" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A33" s="32">
-        <f>B5</f>
-        <v>0.29763539999999999</v>
-      </c>
-      <c r="B33" s="32">
-        <f>D5</f>
-        <v>1.4000000000000012E-2</v>
-      </c>
-      <c r="C33" s="32">
-        <f>F5</f>
-        <v>2.0000000000000018E-2</v>
-      </c>
-      <c r="D33" s="28">
-        <f>$B$26*D5+$C$26</f>
-        <v>1.3625248000000002E-7</v>
-      </c>
-      <c r="E33" s="32">
-        <f>D5/$G$17</f>
-        <v>3.3898305084745797E-2</v>
+      <c r="A33" s="26">
+        <f t="shared" si="7"/>
+        <v>0.19865250000000001</v>
+      </c>
+      <c r="B33" s="26">
+        <f t="shared" si="8"/>
+        <v>6.0000000000000053E-3</v>
+      </c>
+      <c r="C33" s="26">
+        <f t="shared" si="9"/>
+        <v>1.100000000000001E-2</v>
+      </c>
+      <c r="D33" s="22">
+        <f t="shared" si="10"/>
+        <v>1.3842592000000003E-7</v>
+      </c>
+      <c r="E33" s="26">
+        <f t="shared" si="11"/>
+        <v>1.4527845036319625E-2</v>
       </c>
       <c r="F33" s="17">
-        <f>F5/$G$17</f>
-        <v>4.8426150121065423E-2</v>
-      </c>
-      <c r="G33" s="28">
-        <f t="shared" si="5"/>
-        <v>2184440.2391794994</v>
-      </c>
-      <c r="H33" s="28">
-        <f t="shared" ref="H33:H43" si="6">G33/E33</f>
-        <v>64440987.05579517</v>
+        <f t="shared" si="12"/>
+        <v>2.6634382566585981E-2</v>
+      </c>
+      <c r="G33" s="22">
+        <f t="shared" ref="G33:G44" si="13">A33/D33</f>
+        <v>1435081.6667861047</v>
+      </c>
+      <c r="H33" s="22">
+        <f>G33/F33</f>
+        <v>53880793.489332788</v>
       </c>
     </row>
     <row r="34" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A34" s="32">
-        <f>B6</f>
-        <v>0.39720690000000003</v>
-      </c>
-      <c r="B34" s="32">
-        <f>D6</f>
-        <v>2.300000000000002E-2</v>
-      </c>
-      <c r="C34" s="32">
-        <f>F6</f>
-        <v>3.0000000000000027E-2</v>
-      </c>
-      <c r="D34" s="28">
-        <f>$B$26*D6+$C$26</f>
-        <v>1.3380736000000001E-7</v>
-      </c>
-      <c r="E34" s="32">
-        <f>D6/$G$17</f>
-        <v>5.5690072639225235E-2</v>
+      <c r="A34" s="26">
+        <f t="shared" si="7"/>
+        <v>0.29763539999999999</v>
+      </c>
+      <c r="B34" s="26">
+        <f t="shared" si="8"/>
+        <v>1.4000000000000012E-2</v>
+      </c>
+      <c r="C34" s="26">
+        <f t="shared" si="9"/>
+        <v>2.0000000000000018E-2</v>
+      </c>
+      <c r="D34" s="22">
+        <f t="shared" si="10"/>
+        <v>1.3625248000000002E-7</v>
+      </c>
+      <c r="E34" s="26">
+        <f t="shared" si="11"/>
+        <v>3.3898305084745797E-2</v>
       </c>
       <c r="F34" s="17">
-        <f>F6/$G$17</f>
-        <v>7.2639225181598127E-2</v>
-      </c>
-      <c r="G34" s="28">
-        <f t="shared" si="5"/>
-        <v>2968498.1453934968</v>
-      </c>
-      <c r="H34" s="28">
-        <f t="shared" si="6"/>
-        <v>53303901.480326653</v>
+        <f t="shared" si="12"/>
+        <v>4.8426150121065423E-2</v>
+      </c>
+      <c r="G34" s="22">
+        <f t="shared" si="13"/>
+        <v>2184440.2391794994</v>
+      </c>
+      <c r="H34" s="22">
+        <f t="shared" ref="H34:H44" si="14">G34/E34</f>
+        <v>64440987.05579517</v>
       </c>
     </row>
     <row r="35" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A35" s="32">
-        <f>B7</f>
-        <v>0.49599360000000003</v>
-      </c>
-      <c r="B35" s="32">
-        <f>D7</f>
-        <v>3.400000000000003E-2</v>
-      </c>
-      <c r="C35" s="32">
-        <f>F7</f>
-        <v>4.3000000000000038E-2</v>
-      </c>
-      <c r="D35" s="28">
-        <f>$B$26*D7+$C$26</f>
-        <v>1.3081888000000002E-7</v>
-      </c>
-      <c r="E35" s="32">
-        <f>D7/$G$17</f>
-        <v>8.232445520581122E-2</v>
+      <c r="A35" s="26">
+        <f t="shared" si="7"/>
+        <v>0.39720690000000003</v>
+      </c>
+      <c r="B35" s="26">
+        <f t="shared" si="8"/>
+        <v>2.300000000000002E-2</v>
+      </c>
+      <c r="C35" s="26">
+        <f t="shared" si="9"/>
+        <v>3.0000000000000027E-2</v>
+      </c>
+      <c r="D35" s="22">
+        <f t="shared" si="10"/>
+        <v>1.3380736000000001E-7</v>
+      </c>
+      <c r="E35" s="26">
+        <f t="shared" si="11"/>
+        <v>5.5690072639225235E-2</v>
       </c>
       <c r="F35" s="17">
-        <f>F7/$G$17</f>
-        <v>0.10411622276029066</v>
-      </c>
-      <c r="G35" s="28">
-        <f t="shared" si="5"/>
-        <v>3791452.7322050147</v>
-      </c>
-      <c r="H35" s="28">
-        <f t="shared" si="6"/>
-        <v>46054999.364725575</v>
+        <f t="shared" si="12"/>
+        <v>7.2639225181598127E-2</v>
+      </c>
+      <c r="G35" s="22">
+        <f t="shared" si="13"/>
+        <v>2968498.1453934968</v>
+      </c>
+      <c r="H35" s="22">
+        <f t="shared" si="14"/>
+        <v>53303901.480326653</v>
       </c>
     </row>
     <row r="36" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A36" s="32">
-        <f>B8</f>
-        <v>0.59458409999999995</v>
-      </c>
-      <c r="B36" s="32">
-        <f>D8</f>
-        <v>4.500000000000004E-2</v>
-      </c>
-      <c r="C36" s="32">
-        <f>F8</f>
-        <v>5.6999999999999995E-2</v>
-      </c>
-      <c r="D36" s="28">
-        <f>$B$26*D8+$C$26</f>
-        <v>1.278304E-7</v>
-      </c>
-      <c r="E36" s="32">
-        <f>D8/$G$17</f>
-        <v>0.10895883777239719</v>
+      <c r="A36" s="26">
+        <f t="shared" si="7"/>
+        <v>0.49599360000000003</v>
+      </c>
+      <c r="B36" s="26">
+        <f t="shared" si="8"/>
+        <v>3.400000000000003E-2</v>
+      </c>
+      <c r="C36" s="26">
+        <f t="shared" si="9"/>
+        <v>4.3000000000000038E-2</v>
+      </c>
+      <c r="D36" s="22">
+        <f t="shared" si="10"/>
+        <v>1.3081888000000002E-7</v>
+      </c>
+      <c r="E36" s="26">
+        <f t="shared" si="11"/>
+        <v>8.232445520581122E-2</v>
       </c>
       <c r="F36" s="17">
-        <f>F8/$G$17</f>
-        <v>0.13801452784503632</v>
-      </c>
-      <c r="G36" s="28">
-        <f t="shared" si="5"/>
-        <v>4651351.3217513198</v>
-      </c>
-      <c r="H36" s="28">
-        <f t="shared" si="6"/>
-        <v>42689068.797406517</v>
+        <f t="shared" si="12"/>
+        <v>0.10411622276029066</v>
+      </c>
+      <c r="G36" s="22">
+        <f t="shared" si="13"/>
+        <v>3791452.7322050147</v>
+      </c>
+      <c r="H36" s="22">
+        <f t="shared" si="14"/>
+        <v>46054999.364725575</v>
       </c>
     </row>
     <row r="37" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A37" s="32">
-        <f>B9</f>
-        <v>0.6930765000000001</v>
-      </c>
-      <c r="B37" s="32">
-        <f>D9</f>
-        <v>0.06</v>
-      </c>
-      <c r="C37" s="32">
-        <f>F9</f>
-        <v>7.400000000000001E-2</v>
-      </c>
-      <c r="D37" s="28">
-        <f>$B$26*D9+$C$26</f>
-        <v>1.237552E-7</v>
-      </c>
-      <c r="E37" s="32">
-        <f>D9/$G$17</f>
-        <v>0.14527845036319612</v>
+      <c r="A37" s="26">
+        <f t="shared" si="7"/>
+        <v>0.59458409999999995</v>
+      </c>
+      <c r="B37" s="26">
+        <f t="shared" si="8"/>
+        <v>4.500000000000004E-2</v>
+      </c>
+      <c r="C37" s="26">
+        <f t="shared" si="9"/>
+        <v>5.6999999999999995E-2</v>
+      </c>
+      <c r="D37" s="22">
+        <f t="shared" si="10"/>
+        <v>1.278304E-7</v>
+      </c>
+      <c r="E37" s="26">
+        <f t="shared" si="11"/>
+        <v>0.10895883777239719</v>
       </c>
       <c r="F37" s="17">
-        <f>F9/$G$17</f>
-        <v>0.17917675544794193</v>
-      </c>
-      <c r="G37" s="28">
-        <f t="shared" si="5"/>
-        <v>5600382.8525993265</v>
-      </c>
-      <c r="H37" s="28">
-        <f t="shared" si="6"/>
-        <v>38549301.968725368</v>
+        <f t="shared" si="12"/>
+        <v>0.13801452784503632</v>
+      </c>
+      <c r="G37" s="22">
+        <f t="shared" si="13"/>
+        <v>4651351.3217513198</v>
+      </c>
+      <c r="H37" s="22">
+        <f t="shared" si="14"/>
+        <v>42689068.797406517</v>
       </c>
     </row>
     <row r="38" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A38" s="32">
-        <f>B10</f>
-        <v>0.79215750000000007</v>
-      </c>
-      <c r="B38" s="32">
-        <f>D10</f>
-        <v>7.7000000000000013E-2</v>
-      </c>
-      <c r="C38" s="32">
-        <f>F10</f>
-        <v>9.1000000000000025E-2</v>
-      </c>
-      <c r="D38" s="28">
-        <f>$B$26*D10+$C$26</f>
-        <v>1.1913664000000001E-7</v>
-      </c>
-      <c r="E38" s="32">
-        <f>D10/$G$17</f>
-        <v>0.18644067796610173</v>
+      <c r="A38" s="26">
+        <f t="shared" si="7"/>
+        <v>0.6930765000000001</v>
+      </c>
+      <c r="B38" s="26">
+        <f t="shared" si="8"/>
+        <v>0.06</v>
+      </c>
+      <c r="C38" s="26">
+        <f t="shared" si="9"/>
+        <v>7.400000000000001E-2</v>
+      </c>
+      <c r="D38" s="22">
+        <f t="shared" si="10"/>
+        <v>1.237552E-7</v>
+      </c>
+      <c r="E38" s="26">
+        <f t="shared" si="11"/>
+        <v>0.14527845036319612</v>
       </c>
       <c r="F38" s="17">
-        <f>F10/$G$17</f>
-        <v>0.22033898305084754</v>
-      </c>
-      <c r="G38" s="28">
-        <f t="shared" si="5"/>
-        <v>6649150.9245182676</v>
-      </c>
-      <c r="H38" s="28">
-        <f t="shared" si="6"/>
-        <v>35663627.686052524</v>
+        <f t="shared" si="12"/>
+        <v>0.17917675544794193</v>
+      </c>
+      <c r="G38" s="22">
+        <f t="shared" si="13"/>
+        <v>5600382.8525993265</v>
+      </c>
+      <c r="H38" s="22">
+        <f t="shared" si="14"/>
+        <v>38549301.968725368</v>
       </c>
     </row>
     <row r="39" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A39" s="32">
-        <f>B11</f>
-        <v>0.89202329999999996</v>
-      </c>
-      <c r="B39" s="32">
-        <f>D11</f>
-        <v>9.4000000000000028E-2</v>
-      </c>
-      <c r="C39" s="32">
-        <f>F11</f>
-        <v>0.10600000000000004</v>
-      </c>
-      <c r="D39" s="28">
-        <f>$B$26*D11+$C$26</f>
-        <v>1.1451807999999999E-7</v>
-      </c>
-      <c r="E39" s="32">
-        <f>D11/$G$17</f>
-        <v>0.22760290556900734</v>
+      <c r="A39" s="26">
+        <f t="shared" si="7"/>
+        <v>0.79215750000000007</v>
+      </c>
+      <c r="B39" s="26">
+        <f t="shared" si="8"/>
+        <v>7.7000000000000013E-2</v>
+      </c>
+      <c r="C39" s="26">
+        <f t="shared" si="9"/>
+        <v>9.1000000000000025E-2</v>
+      </c>
+      <c r="D39" s="22">
+        <f t="shared" si="10"/>
+        <v>1.1913664000000001E-7</v>
+      </c>
+      <c r="E39" s="26">
+        <f t="shared" si="11"/>
+        <v>0.18644067796610173</v>
       </c>
       <c r="F39" s="17">
-        <f>F11/$G$17</f>
-        <v>0.25665859564164661</v>
-      </c>
-      <c r="G39" s="28">
-        <f t="shared" si="5"/>
-        <v>7789366.5349611174</v>
-      </c>
-      <c r="H39" s="28">
-        <f t="shared" si="6"/>
-        <v>34223493.392967455</v>
+        <f t="shared" si="12"/>
+        <v>0.22033898305084754</v>
+      </c>
+      <c r="G39" s="22">
+        <f t="shared" si="13"/>
+        <v>6649150.9245182676</v>
+      </c>
+      <c r="H39" s="22">
+        <f t="shared" si="14"/>
+        <v>35663627.686052524</v>
       </c>
     </row>
     <row r="40" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A40" s="32">
-        <f>B12</f>
-        <v>0.99051570000000011</v>
-      </c>
-      <c r="B40" s="32">
-        <f>D12</f>
-        <v>0.11600000000000005</v>
-      </c>
-      <c r="C40" s="32">
-        <f>F12</f>
-        <v>0.12600000000000006</v>
-      </c>
-      <c r="D40" s="28">
-        <f>$B$26*D12+$C$26</f>
-        <v>1.0854111999999998E-7</v>
-      </c>
-      <c r="E40" s="32">
-        <f>D12/$G$17</f>
-        <v>0.28087167070217933</v>
+      <c r="A40" s="26">
+        <f t="shared" si="7"/>
+        <v>0.89202329999999996</v>
+      </c>
+      <c r="B40" s="26">
+        <f t="shared" si="8"/>
+        <v>9.4000000000000028E-2</v>
+      </c>
+      <c r="C40" s="26">
+        <f t="shared" si="9"/>
+        <v>0.10600000000000004</v>
+      </c>
+      <c r="D40" s="22">
+        <f t="shared" si="10"/>
+        <v>1.1451807999999999E-7</v>
+      </c>
+      <c r="E40" s="26">
+        <f t="shared" si="11"/>
+        <v>0.22760290556900734</v>
       </c>
       <c r="F40" s="17">
-        <f>F12/$G$17</f>
-        <v>0.305084745762712</v>
-      </c>
-      <c r="G40" s="28">
-        <f t="shared" si="5"/>
-        <v>9125718.4373995792</v>
-      </c>
-      <c r="H40" s="28">
-        <f t="shared" si="6"/>
-        <v>32490704.436603658</v>
+        <f t="shared" si="12"/>
+        <v>0.25665859564164661</v>
+      </c>
+      <c r="G40" s="22">
+        <f t="shared" si="13"/>
+        <v>7789366.5349611174</v>
+      </c>
+      <c r="H40" s="22">
+        <f t="shared" si="14"/>
+        <v>34223493.392967455</v>
       </c>
     </row>
     <row r="41" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A41" s="32">
-        <f>B13</f>
-        <v>1.0892043</v>
-      </c>
-      <c r="B41" s="32">
-        <f>D13</f>
-        <v>0.13400000000000006</v>
-      </c>
-      <c r="C41" s="32">
-        <f>F13</f>
-        <v>0.14600000000000007</v>
-      </c>
-      <c r="D41" s="28">
-        <f>$B$26*D13+$C$26</f>
-        <v>1.0365087999999997E-7</v>
-      </c>
-      <c r="E41" s="32">
-        <f>D13/$G$17</f>
-        <v>0.32445520581113818</v>
+      <c r="A41" s="26">
+        <f t="shared" si="7"/>
+        <v>0.99051570000000011</v>
+      </c>
+      <c r="B41" s="26">
+        <f t="shared" si="8"/>
+        <v>0.11600000000000005</v>
+      </c>
+      <c r="C41" s="26">
+        <f t="shared" si="9"/>
+        <v>0.12600000000000006</v>
+      </c>
+      <c r="D41" s="22">
+        <f t="shared" si="10"/>
+        <v>1.0854111999999998E-7</v>
+      </c>
+      <c r="E41" s="26">
+        <f t="shared" si="11"/>
+        <v>0.28087167070217933</v>
       </c>
       <c r="F41" s="17">
-        <f>F13/$G$17</f>
-        <v>0.35351089588377743</v>
-      </c>
-      <c r="G41" s="28">
-        <f t="shared" si="5"/>
-        <v>10508394.140020812</v>
-      </c>
-      <c r="H41" s="28">
-        <f t="shared" si="6"/>
-        <v>32387811.789765619</v>
+        <f t="shared" si="12"/>
+        <v>0.305084745762712</v>
+      </c>
+      <c r="G41" s="22">
+        <f t="shared" si="13"/>
+        <v>9125718.4373995792</v>
+      </c>
+      <c r="H41" s="22">
+        <f t="shared" si="14"/>
+        <v>32490704.436603658</v>
       </c>
     </row>
     <row r="42" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A42" s="32">
-        <f>B14</f>
-        <v>1.1877948</v>
-      </c>
-      <c r="B42" s="32">
-        <f>D14</f>
-        <v>0.15599999999999997</v>
-      </c>
-      <c r="C42" s="32">
-        <f>F14</f>
-        <v>0.16299999999999998</v>
-      </c>
-      <c r="D42" s="28">
-        <f>$B$26*D14+$C$26</f>
-        <v>9.7673919999999993E-8</v>
-      </c>
-      <c r="E42" s="32">
-        <f>D14/$G$17</f>
-        <v>0.37772397094430987</v>
+      <c r="A42" s="26">
+        <f t="shared" si="7"/>
+        <v>1.0892043</v>
+      </c>
+      <c r="B42" s="26">
+        <f t="shared" si="8"/>
+        <v>0.13400000000000006</v>
+      </c>
+      <c r="C42" s="26">
+        <f t="shared" si="9"/>
+        <v>0.14600000000000007</v>
+      </c>
+      <c r="D42" s="22">
+        <f t="shared" si="10"/>
+        <v>1.0365087999999997E-7</v>
+      </c>
+      <c r="E42" s="26">
+        <f t="shared" si="11"/>
+        <v>0.32445520581113818</v>
       </c>
       <c r="F42" s="17">
-        <f>F14/$G$17</f>
-        <v>0.39467312348668276</v>
-      </c>
-      <c r="G42" s="28">
-        <f t="shared" si="5"/>
-        <v>12160818.363796601</v>
-      </c>
-      <c r="H42" s="28">
-        <f t="shared" si="6"/>
-        <v>32194987.078512803</v>
+        <f t="shared" si="12"/>
+        <v>0.35351089588377743</v>
+      </c>
+      <c r="G42" s="22">
+        <f t="shared" si="13"/>
+        <v>10508394.140020812</v>
+      </c>
+      <c r="H42" s="22">
+        <f t="shared" si="14"/>
+        <v>32387811.789765619</v>
       </c>
     </row>
     <row r="43" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A43" s="32">
-        <f>B15</f>
-        <v>1.2876605999999999</v>
-      </c>
-      <c r="B43" s="32">
-        <f>D15</f>
-        <v>0.17499999999999999</v>
-      </c>
-      <c r="C43" s="32">
-        <f>F15</f>
-        <v>0.17699999999999999</v>
-      </c>
-      <c r="D43" s="28">
-        <f>$B$26*D15+$C$26</f>
-        <v>9.2511999999999975E-8</v>
-      </c>
-      <c r="E43" s="32">
-        <f>D15/$G$17</f>
-        <v>0.42372881355932202</v>
+      <c r="A43" s="26">
+        <f t="shared" si="7"/>
+        <v>1.1877948</v>
+      </c>
+      <c r="B43" s="26">
+        <f t="shared" si="8"/>
+        <v>0.15599999999999997</v>
+      </c>
+      <c r="C43" s="26">
+        <f t="shared" si="9"/>
+        <v>0.16299999999999998</v>
+      </c>
+      <c r="D43" s="22">
+        <f t="shared" si="10"/>
+        <v>9.7673919999999993E-8</v>
+      </c>
+      <c r="E43" s="26">
+        <f t="shared" si="11"/>
+        <v>0.37772397094430987</v>
       </c>
       <c r="F43" s="17">
-        <f>F15/$G$17</f>
-        <v>0.42857142857142855</v>
-      </c>
-      <c r="G43" s="28">
-        <f t="shared" si="5"/>
-        <v>13918849.446558287</v>
-      </c>
-      <c r="H43" s="28">
-        <f t="shared" si="6"/>
-        <v>32848484.693877559</v>
+        <f t="shared" si="12"/>
+        <v>0.39467312348668276</v>
+      </c>
+      <c r="G43" s="22">
+        <f t="shared" si="13"/>
+        <v>12160818.363796601</v>
+      </c>
+      <c r="H43" s="22">
+        <f t="shared" si="14"/>
+        <v>32194987.078512803</v>
       </c>
     </row>
     <row r="44" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="Q44" s="7"/>
-      <c r="R44" s="7"/>
-      <c r="S44" s="7"/>
-      <c r="T44" s="7"/>
-      <c r="U44" s="7"/>
-      <c r="V44" s="7"/>
-      <c r="W44" s="7"/>
-      <c r="X44" s="7"/>
-      <c r="Y44" s="7"/>
-      <c r="Z44" s="7"/>
-      <c r="AA44" s="7"/>
-      <c r="AB44" s="7"/>
-      <c r="AC44" s="7"/>
-      <c r="AD44" s="7"/>
-      <c r="AE44" s="7"/>
+      <c r="A44" s="26">
+        <f t="shared" si="7"/>
+        <v>1.2876605999999999</v>
+      </c>
+      <c r="B44" s="26">
+        <f t="shared" si="8"/>
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="C44" s="26">
+        <f t="shared" si="9"/>
+        <v>0.17699999999999999</v>
+      </c>
+      <c r="D44" s="22">
+        <f t="shared" si="10"/>
+        <v>9.2511999999999975E-8</v>
+      </c>
+      <c r="E44" s="26">
+        <f t="shared" si="11"/>
+        <v>0.42372881355932202</v>
+      </c>
+      <c r="F44" s="17">
+        <f t="shared" si="12"/>
+        <v>0.42857142857142855</v>
+      </c>
+      <c r="G44" s="22">
+        <f t="shared" si="13"/>
+        <v>13918849.446558287</v>
+      </c>
+      <c r="H44" s="22">
+        <f t="shared" si="14"/>
+        <v>32848484.693877559</v>
+      </c>
+    </row>
+    <row r="45" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="Q45" s="7"/>
+      <c r="R45" s="7"/>
+      <c r="S45" s="7"/>
+      <c r="T45" s="7"/>
+      <c r="U45" s="7"/>
+      <c r="V45" s="7"/>
+      <c r="W45" s="7"/>
+      <c r="X45" s="7"/>
+      <c r="Y45" s="7"/>
+      <c r="Z45" s="7"/>
+      <c r="AA45" s="7"/>
+      <c r="AB45" s="7"/>
+      <c r="AC45" s="7"/>
+      <c r="AD45" s="7"/>
+      <c r="AE45" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="9">
     <mergeCell ref="X1:Y1"/>
     <mergeCell ref="Z1:AA1"/>
-    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="D29:E29"/>
     <mergeCell ref="D28:E28"/>
     <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D26:E26"/>
     <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="A21:D21"/>
+    <mergeCell ref="A18:D18"/>
+    <mergeCell ref="A22:D22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -16862,24 +16871,24 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="AE2" s="20" t="s">
+      <c r="AE2" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="AF2" s="20"/>
-      <c r="AG2" s="20" t="s">
+      <c r="AF2" s="29"/>
+      <c r="AG2" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="AH2" s="20"/>
+      <c r="AH2" s="29"/>
     </row>
     <row r="3" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="26"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="37"/>
       <c r="AE3" s="6" t="s">
         <v>13</v>
       </c>
@@ -16912,526 +16921,526 @@
       <c r="F4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="AE4" s="30">
+      <c r="AE4" s="24">
         <f>$S$19*F6+$T$19</f>
         <v>-3.5879173083905704</v>
       </c>
-      <c r="AF4" s="30">
+      <c r="AF4" s="24">
         <f>E6-AE4</f>
         <v>-0.34390832433375484</v>
       </c>
-      <c r="AG4" s="30">
+      <c r="AG4" s="24">
         <f>$S$39*F26+$T$39</f>
         <v>-5.5813988687434586</v>
       </c>
-      <c r="AH4" s="30">
+      <c r="AH4" s="24">
         <f>E26-AG4</f>
         <v>5.9937950881213453E-2</v>
       </c>
     </row>
     <row r="5" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A5" s="27">
+      <c r="A5" s="35">
         <v>9.0939999999999993E-2</v>
       </c>
-      <c r="B5" s="29">
+      <c r="B5" s="23">
         <v>0.51500000000000001</v>
       </c>
-      <c r="C5" s="29">
-        <f>B5-'Carga e Descarga'!$G$17</f>
+      <c r="C5" s="23">
+        <f>B5-'Carga e Descarga'!$G$18</f>
         <v>0.10200000000000004</v>
       </c>
-      <c r="D5" s="29">
+      <c r="D5" s="23">
         <f t="shared" ref="D5:D21" si="0">C5/$P$18</f>
         <v>0.24697336561743352</v>
       </c>
       <c r="E5" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="34">
+      <c r="F5" s="28">
         <v>30</v>
       </c>
-      <c r="AE5" s="30">
+      <c r="AE5" s="24">
         <f t="shared" ref="AE5:AE16" si="1">$S$19*F7+$T$19</f>
         <v>-3.5496565606661639</v>
       </c>
-      <c r="AF5" s="30">
+      <c r="AF5" s="24">
         <f t="shared" ref="AF5:AF16" si="2">E7-AE5</f>
         <v>2.3296036050003188E-2</v>
       </c>
-      <c r="AG5" s="30">
+      <c r="AG5" s="24">
         <f t="shared" ref="AG5:AG16" si="3">$S$39*F27+$T$39</f>
         <v>-5.6208686979581248</v>
       </c>
-      <c r="AH5" s="30">
+      <c r="AH5" s="24">
         <f t="shared" ref="AH5:AH16" si="4">E27-AG5</f>
         <v>7.4089972111591962E-2</v>
       </c>
     </row>
     <row r="6" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A6" s="25"/>
-      <c r="B6" s="29">
+      <c r="A6" s="36"/>
+      <c r="B6" s="23">
         <v>0.51700000000000002</v>
       </c>
-      <c r="C6" s="29">
-        <f>B6-'Carga e Descarga'!$G$17</f>
+      <c r="C6" s="23">
+        <f>B6-'Carga e Descarga'!$G$18</f>
         <v>0.10400000000000004</v>
       </c>
-      <c r="D6" s="29">
+      <c r="D6" s="23">
         <f t="shared" si="0"/>
         <v>0.25181598062954008</v>
       </c>
-      <c r="E6" s="29">
+      <c r="E6" s="23">
         <f>LN((-$C$5+C6)/$C$5)</f>
         <v>-3.9318256327243253</v>
       </c>
-      <c r="F6" s="34">
+      <c r="F6" s="28">
         <v>80</v>
       </c>
-      <c r="AE6" s="30">
+      <c r="AE6" s="24">
         <f t="shared" si="1"/>
         <v>-3.5205451221802022</v>
       </c>
-      <c r="AF6" s="30">
+      <c r="AF6" s="24">
         <f t="shared" si="2"/>
         <v>5.8723118701605515E-2</v>
       </c>
-      <c r="AG6" s="30">
+      <c r="AG6" s="24">
         <f t="shared" si="3"/>
         <v>-5.6499125345500492</v>
       </c>
-      <c r="AH6" s="30">
+      <c r="AH6" s="24">
         <f t="shared" si="4"/>
         <v>-5.0797759367187112E-3</v>
       </c>
     </row>
     <row r="7" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A7" s="25"/>
-      <c r="B7" s="29">
+      <c r="A7" s="36"/>
+      <c r="B7" s="23">
         <v>0.51800000000000002</v>
       </c>
-      <c r="C7" s="29">
-        <f>B7-'Carga e Descarga'!$G$17</f>
+      <c r="C7" s="23">
+        <f>B7-'Carga e Descarga'!$G$18</f>
         <v>0.10500000000000004</v>
       </c>
-      <c r="D7" s="29">
+      <c r="D7" s="23">
         <f t="shared" si="0"/>
         <v>0.25423728813559332</v>
       </c>
-      <c r="E7" s="29">
+      <c r="E7" s="23">
         <f t="shared" ref="E7:E21" si="5">LN((-$C$5+C7)/$C$5)</f>
         <v>-3.5263605246161607</v>
       </c>
-      <c r="F7" s="34">
+      <c r="F7" s="28">
         <v>126</v>
       </c>
-      <c r="AE7" s="30">
+      <c r="AE7" s="24">
         <f t="shared" si="1"/>
         <v>-3.4839478852264216</v>
       </c>
-      <c r="AF7" s="30">
+      <c r="AF7" s="24">
         <f t="shared" si="2"/>
         <v>-0.11140551087668271</v>
       </c>
-      <c r="AG7" s="30">
+      <c r="AG7" s="24">
         <f t="shared" si="3"/>
         <v>-5.6819352261770426</v>
       </c>
-      <c r="AH7" s="30">
+      <c r="AH7" s="24">
         <f t="shared" si="4"/>
         <v>-2.0446211829749927E-3</v>
       </c>
     </row>
     <row r="8" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A8" s="25"/>
-      <c r="B8" s="29">
+      <c r="A8" s="36"/>
+      <c r="B8" s="23">
         <v>0.51819999999999999</v>
       </c>
-      <c r="C8" s="29">
-        <f>B8-'Carga e Descarga'!$G$17</f>
+      <c r="C8" s="23">
+        <f>B8-'Carga e Descarga'!$G$18</f>
         <v>0.10520000000000002</v>
       </c>
-      <c r="D8" s="29">
+      <c r="D8" s="23">
         <f t="shared" si="0"/>
         <v>0.25472154963680393</v>
       </c>
-      <c r="E8" s="29">
+      <c r="E8" s="23">
         <f t="shared" si="5"/>
         <v>-3.4618220034785967</v>
       </c>
-      <c r="F8" s="34">
+      <c r="F8" s="28">
         <v>161</v>
       </c>
-      <c r="AE8" s="30">
+      <c r="AE8" s="24">
         <f t="shared" si="1"/>
         <v>-3.4465188928873283</v>
       </c>
-      <c r="AF8" s="30">
+      <c r="AF8" s="24">
         <f t="shared" si="2"/>
         <v>7.4309048098410102E-2</v>
       </c>
-      <c r="AG8" s="30">
+      <c r="AG8" s="24">
         <f t="shared" si="3"/>
         <v>-5.7325757617732185</v>
       </c>
-      <c r="AH8" s="30">
+      <c r="AH8" s="24">
         <f t="shared" si="4"/>
         <v>1.8742951263523544E-2</v>
       </c>
     </row>
     <row r="9" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A9" s="25"/>
-      <c r="B9" s="29">
+      <c r="A9" s="36"/>
+      <c r="B9" s="23">
         <v>0.51780000000000004</v>
       </c>
-      <c r="C9" s="29">
-        <f>B9-'Carga e Descarga'!$G$17</f>
+      <c r="C9" s="23">
+        <f>B9-'Carga e Descarga'!$G$18</f>
         <v>0.10480000000000006</v>
       </c>
-      <c r="D9" s="29">
+      <c r="D9" s="23">
         <f t="shared" si="0"/>
         <v>0.25375302663438271</v>
       </c>
-      <c r="E9" s="29">
+      <c r="E9" s="23">
         <f t="shared" si="5"/>
         <v>-3.5953533961031043</v>
       </c>
-      <c r="F9" s="34">
+      <c r="F9" s="28">
         <v>205</v>
       </c>
-      <c r="AE9" s="30">
+      <c r="AE9" s="24">
         <f t="shared" si="1"/>
         <v>-3.4007723466951028</v>
       </c>
-      <c r="AF9" s="30">
+      <c r="AF9" s="24">
         <f t="shared" si="2"/>
         <v>8.4132353061019849E-2</v>
       </c>
-      <c r="AG9" s="30">
+      <c r="AG9" s="24">
         <f t="shared" si="3"/>
         <v>-5.7802374423343252</v>
       </c>
-      <c r="AH9" s="30">
+      <c r="AH9" s="24">
         <f t="shared" si="4"/>
         <v>-2.8905547979701574E-2</v>
       </c>
     </row>
     <row r="10" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A10" s="25"/>
-      <c r="B10" s="29">
+      <c r="A10" s="36"/>
+      <c r="B10" s="23">
         <v>0.51849999999999996</v>
       </c>
-      <c r="C10" s="29">
-        <f>B10-'Carga e Descarga'!$G$17</f>
+      <c r="C10" s="23">
+        <f>B10-'Carga e Descarga'!$G$18</f>
         <v>0.10549999999999998</v>
       </c>
-      <c r="D10" s="29">
+      <c r="D10" s="23">
         <f t="shared" si="0"/>
         <v>0.2554479418886198</v>
       </c>
-      <c r="E10" s="29">
+      <c r="E10" s="23">
         <f t="shared" si="5"/>
         <v>-3.3722098447889182</v>
       </c>
-      <c r="F10" s="34">
+      <c r="F10" s="28">
         <v>250</v>
       </c>
-      <c r="AE10" s="30">
+      <c r="AE10" s="24">
         <f t="shared" si="1"/>
         <v>-3.3076157435400253</v>
       </c>
-      <c r="AF10" s="30">
+      <c r="AF10" s="24">
         <f t="shared" si="2"/>
         <v>9.3629903966014005E-2</v>
       </c>
-      <c r="AG10" s="30">
+      <c r="AG10" s="24">
         <f t="shared" si="3"/>
         <v>-5.8301332641717334</v>
       </c>
-      <c r="AH10" s="30">
+      <c r="AH10" s="24">
         <f t="shared" si="4"/>
         <v>-8.4370241800106882E-2</v>
       </c>
     </row>
     <row r="11" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A11" s="25"/>
-      <c r="B11" s="29">
+      <c r="A11" s="36"/>
+      <c r="B11" s="23">
         <v>0.51870000000000005</v>
       </c>
-      <c r="C11" s="29">
-        <f>B11-'Carga e Descarga'!$G$17</f>
+      <c r="C11" s="23">
+        <f>B11-'Carga e Descarga'!$G$18</f>
         <v>0.10570000000000007</v>
       </c>
-      <c r="D11" s="29">
+      <c r="D11" s="23">
         <f t="shared" si="0"/>
         <v>0.25593220338983069</v>
       </c>
-      <c r="E11" s="29">
+      <c r="E11" s="23">
         <f t="shared" si="5"/>
         <v>-3.3166399936340829</v>
       </c>
-      <c r="F11" s="34">
+      <c r="F11" s="28">
         <v>305</v>
       </c>
-      <c r="AE11" s="30">
+      <c r="AE11" s="24">
         <f t="shared" si="1"/>
         <v>-3.2618691973477998</v>
       </c>
-      <c r="AF11" s="30">
+      <c r="AF11" s="24">
         <f t="shared" si="2"/>
         <v>0.14097378083979084</v>
       </c>
-      <c r="AG11" s="30">
+      <c r="AG11" s="24">
         <f t="shared" si="3"/>
         <v>-5.9060940675659968</v>
       </c>
-      <c r="AH11" s="30">
+      <c r="AH11" s="24">
         <f t="shared" si="4"/>
         <v>-4.614976638868562E-2</v>
       </c>
     </row>
     <row r="12" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A12" s="25"/>
-      <c r="B12" s="29">
+      <c r="A12" s="36"/>
+      <c r="B12" s="23">
         <v>0.51910000000000001</v>
       </c>
-      <c r="C12" s="29">
-        <f>B12-'Carga e Descarga'!$G$17</f>
+      <c r="C12" s="23">
+        <f>B12-'Carga e Descarga'!$G$18</f>
         <v>0.10610000000000003</v>
       </c>
-      <c r="D12" s="29">
+      <c r="D12" s="23">
         <f t="shared" si="0"/>
         <v>0.25690072639225192</v>
       </c>
-      <c r="E12" s="29">
+      <c r="E12" s="23">
         <f t="shared" si="5"/>
         <v>-3.2139858395740113</v>
       </c>
-      <c r="F12" s="34">
+      <c r="F12" s="28">
         <v>417</v>
       </c>
-      <c r="AE12" s="30">
+      <c r="AE12" s="24">
         <f t="shared" si="1"/>
         <v>-3.2086368526877553</v>
       </c>
-      <c r="AF12" s="30">
+      <c r="AF12" s="24">
         <f t="shared" si="2"/>
         <v>8.774143617974639E-2</v>
       </c>
-      <c r="AG12" s="30">
+      <c r="AG12" s="24">
         <f t="shared" si="3"/>
         <v>-5.975352447131355</v>
       </c>
-      <c r="AH12" s="30">
+      <c r="AH12" s="24">
         <f t="shared" si="4"/>
         <v>-1.6112099976625771E-2</v>
       </c>
     </row>
     <row r="13" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A13" s="25"/>
-      <c r="B13" s="29">
+      <c r="A13" s="36"/>
+      <c r="B13" s="23">
         <v>0.51949999999999996</v>
       </c>
-      <c r="C13" s="29">
-        <f>B13-'Carga e Descarga'!$G$17</f>
+      <c r="C13" s="23">
+        <f>B13-'Carga e Descarga'!$G$18</f>
         <v>0.10649999999999998</v>
       </c>
-      <c r="D13" s="29">
+      <c r="D13" s="23">
         <f t="shared" si="0"/>
         <v>0.25786924939467309</v>
       </c>
-      <c r="E13" s="29">
+      <c r="E13" s="23">
         <f t="shared" si="5"/>
         <v>-3.1208954165080089</v>
       </c>
-      <c r="F13" s="34">
+      <c r="F13" s="28">
         <v>472</v>
       </c>
-      <c r="AE13" s="30">
+      <c r="AE13" s="24">
         <f t="shared" si="1"/>
         <v>-3.1603950403395906</v>
       </c>
-      <c r="AF13" s="30">
+      <c r="AF13" s="24">
         <f t="shared" si="2"/>
         <v>0.10403814496917008</v>
       </c>
-      <c r="AG13" s="30">
+      <c r="AG13" s="24">
         <f t="shared" si="3"/>
         <v>-6.0505685367668516</v>
       </c>
-      <c r="AH13" s="30">
+      <c r="AH13" s="24">
         <f t="shared" si="4"/>
         <v>-6.8729381850999083E-2</v>
       </c>
     </row>
     <row r="14" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A14" s="25"/>
-      <c r="B14" s="29">
+      <c r="A14" s="36"/>
+      <c r="B14" s="23">
         <v>0.51949999999999996</v>
       </c>
-      <c r="C14" s="29">
-        <f>B14-'Carga e Descarga'!$G$17</f>
+      <c r="C14" s="23">
+        <f>B14-'Carga e Descarga'!$G$18</f>
         <v>0.10649999999999998</v>
       </c>
-      <c r="D14" s="29">
+      <c r="D14" s="23">
         <f t="shared" si="0"/>
         <v>0.25786924939467309</v>
       </c>
-      <c r="E14" s="29">
+      <c r="E14" s="23">
         <f t="shared" si="5"/>
         <v>-3.1208954165080089</v>
       </c>
-      <c r="F14" s="34">
+      <c r="F14" s="28">
         <v>536</v>
       </c>
-      <c r="AE14" s="30">
+      <c r="AE14" s="24">
         <f t="shared" si="1"/>
         <v>-3.1121532279914255</v>
       </c>
-      <c r="AF14" s="30">
+      <c r="AF14" s="24">
         <f t="shared" si="2"/>
         <v>7.6415619823738012E-2</v>
       </c>
-      <c r="AG14" s="30">
+      <c r="AG14" s="24">
         <f t="shared" si="3"/>
         <v>-6.1302529089549509</v>
       </c>
-      <c r="AH14" s="30">
+      <c r="AH14" s="24">
         <f t="shared" si="4"/>
         <v>-3.5565025297787045E-2</v>
       </c>
     </row>
     <row r="15" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A15" s="25"/>
-      <c r="B15" s="29">
+      <c r="A15" s="36"/>
+      <c r="B15" s="23">
         <v>0.51980000000000004</v>
       </c>
-      <c r="C15" s="29">
-        <f>B15-'Carga e Descarga'!$G$17</f>
+      <c r="C15" s="23">
+        <f>B15-'Carga e Descarga'!$G$18</f>
         <v>0.10680000000000006</v>
       </c>
-      <c r="D15" s="29">
+      <c r="D15" s="23">
         <f t="shared" si="0"/>
         <v>0.25859564164648929</v>
       </c>
-      <c r="E15" s="29">
+      <c r="E15" s="23">
         <f t="shared" si="5"/>
         <v>-3.0563568953704205</v>
       </c>
-      <c r="F15" s="34">
+      <c r="F15" s="28">
         <v>594</v>
       </c>
-      <c r="AE15" s="30">
+      <c r="AE15" s="24">
         <f t="shared" si="1"/>
         <v>-3.0647431710285735</v>
       </c>
-      <c r="AF15" s="30">
+      <c r="AF15" s="24">
         <f t="shared" si="2"/>
         <v>4.9208270178403346E-2</v>
       </c>
-      <c r="AG15" s="30">
+      <c r="AG15" s="24">
         <f t="shared" si="3"/>
         <v>-6.2121714224193534</v>
       </c>
-      <c r="AH15" s="30">
+      <c r="AH15" s="24">
         <f t="shared" si="4"/>
         <v>-2.4366760028371459E-3</v>
       </c>
     </row>
     <row r="16" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A16" s="25"/>
-      <c r="B16" s="29">
+      <c r="A16" s="36"/>
+      <c r="B16" s="23">
         <v>0.51990000000000003</v>
       </c>
-      <c r="C16" s="29">
-        <f>B16-'Carga e Descarga'!$G$17</f>
+      <c r="C16" s="23">
+        <f>B16-'Carga e Descarga'!$G$18</f>
         <v>0.10690000000000005</v>
       </c>
-      <c r="D16" s="29">
+      <c r="D16" s="23">
         <f t="shared" si="0"/>
         <v>0.25883777239709455</v>
       </c>
-      <c r="E16" s="29">
+      <c r="E16" s="23">
         <f t="shared" si="5"/>
         <v>-3.0357376081676875</v>
       </c>
-      <c r="F16" s="34">
+      <c r="F16" s="28">
         <v>652</v>
       </c>
       <c r="R16">
         <v>9</v>
       </c>
-      <c r="AE16" s="30">
+      <c r="AE16" s="24">
         <f t="shared" si="1"/>
         <v>-3.0023615171300841</v>
       </c>
-      <c r="AF16" s="30">
+      <c r="AF16" s="24">
         <f t="shared" si="2"/>
         <v>-1.3173383720086029E-2</v>
       </c>
-      <c r="AG16" s="30">
+      <c r="AG16" s="24">
         <f t="shared" si="3"/>
         <v>-6.2702590956032012</v>
       </c>
-      <c r="AH16" s="30">
+      <c r="AH16" s="24">
         <f t="shared" si="4"/>
         <v>5.5650997181010631E-2</v>
       </c>
     </row>
     <row r="17" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A17" s="25"/>
-      <c r="B17" s="29">
+      <c r="A17" s="36"/>
+      <c r="B17" s="23">
         <v>0.52</v>
       </c>
-      <c r="C17" s="29">
-        <f>B17-'Carga e Descarga'!$G$17</f>
+      <c r="C17" s="23">
+        <f>B17-'Carga e Descarga'!$G$18</f>
         <v>0.10700000000000004</v>
       </c>
-      <c r="D17" s="29">
+      <c r="D17" s="23">
         <f t="shared" si="0"/>
         <v>0.25907990314769985</v>
       </c>
-      <c r="E17" s="29">
+      <c r="E17" s="23">
         <f t="shared" si="5"/>
         <v>-3.0155349008501702</v>
       </c>
-      <c r="F17" s="34">
+      <c r="F17" s="28">
         <v>709</v>
       </c>
-      <c r="AE17" s="30">
+      <c r="AE17" s="24">
         <f>$S$19*F19+$T$19</f>
         <v>-2.9516244386259798</v>
       </c>
-      <c r="AF17" s="30">
+      <c r="AF17" s="24">
         <f>E19-AE17</f>
         <v>-6.391046222419039E-2</v>
       </c>
-      <c r="AG17" s="30">
+      <c r="AG17" s="24">
         <f>$S$39*F39+$T$39</f>
         <v>-6.2955793634012895</v>
       </c>
-      <c r="AH17" s="30">
+      <c r="AH17" s="24">
         <f>E39-AG17</f>
         <v>8.0971264979099011E-2</v>
       </c>
     </row>
     <row r="18" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A18" s="25"/>
-      <c r="B18" s="29">
+      <c r="A18" s="36"/>
+      <c r="B18" s="23">
         <v>0.52</v>
       </c>
-      <c r="C18" s="29">
-        <f>B18-'Carga e Descarga'!$G$17</f>
+      <c r="C18" s="23">
+        <f>B18-'Carga e Descarga'!$G$18</f>
         <v>0.10700000000000004</v>
       </c>
-      <c r="D18" s="29">
+      <c r="D18" s="23">
         <f t="shared" si="0"/>
         <v>0.25907990314769985</v>
       </c>
-      <c r="E18" s="29">
+      <c r="E18" s="23">
         <f t="shared" si="5"/>
         <v>-3.0155349008501702</v>
       </c>
-      <c r="F18" s="34">
+      <c r="F18" s="28">
         <v>784</v>
       </c>
       <c r="O18" s="1" t="s">
@@ -17440,40 +17449,40 @@
       <c r="P18" s="10">
         <v>0.41299999999999998</v>
       </c>
-      <c r="S18" s="21" t="s">
+      <c r="S18" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="T18" s="21"/>
-      <c r="AE18" s="30">
+      <c r="T18" s="30"/>
+      <c r="AE18" s="24">
         <f t="shared" ref="AE18:AE19" si="6">$S$19*F20+$T$19</f>
         <v>-2.9017191155071882</v>
       </c>
-      <c r="AF18" s="30">
+      <c r="AF18" s="24">
         <f t="shared" ref="AF18:AF19" si="7">E20-AE18</f>
         <v>-0.11381578534298198</v>
       </c>
     </row>
     <row r="19" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A19" s="25"/>
-      <c r="B19" s="29">
+      <c r="A19" s="36"/>
+      <c r="B19" s="23">
         <v>0.52</v>
       </c>
-      <c r="C19" s="29">
-        <f>B19-'Carga e Descarga'!$G$17</f>
+      <c r="C19" s="23">
+        <f>B19-'Carga e Descarga'!$G$18</f>
         <v>0.10700000000000004</v>
       </c>
-      <c r="D19" s="29">
+      <c r="D19" s="23">
         <f t="shared" si="0"/>
         <v>0.25907990314769985</v>
       </c>
-      <c r="E19" s="29">
+      <c r="E19" s="23">
         <f t="shared" si="5"/>
         <v>-3.0155349008501702</v>
       </c>
-      <c r="F19" s="34">
+      <c r="F19" s="28">
         <v>845</v>
       </c>
-      <c r="R19" s="31" t="s">
+      <c r="R19" s="25" t="s">
         <v>36</v>
       </c>
       <c r="S19" s="4">
@@ -17483,15 +17492,15 @@
       <c r="T19" s="4">
         <v>-3.6544577392156259</v>
       </c>
-      <c r="U19" s="22" t="s">
+      <c r="U19" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="V19" s="21"/>
-      <c r="AE19" s="30">
+      <c r="V19" s="30"/>
+      <c r="AE19" s="24">
         <f t="shared" si="6"/>
         <v>-2.8692806554799737</v>
       </c>
-      <c r="AF19" s="30">
+      <c r="AF19" s="24">
         <f t="shared" si="7"/>
         <v>-0.14625424537019649</v>
       </c>
@@ -17499,26 +17508,26 @@
       <c r="AH19" s="15"/>
     </row>
     <row r="20" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A20" s="25"/>
-      <c r="B20" s="29">
+      <c r="A20" s="36"/>
+      <c r="B20" s="23">
         <v>0.52</v>
       </c>
-      <c r="C20" s="29">
-        <f>B20-'Carga e Descarga'!$G$17</f>
+      <c r="C20" s="23">
+        <f>B20-'Carga e Descarga'!$G$18</f>
         <v>0.10700000000000004</v>
       </c>
-      <c r="D20" s="29">
+      <c r="D20" s="23">
         <f t="shared" si="0"/>
         <v>0.25907990314769985</v>
       </c>
-      <c r="E20" s="29">
+      <c r="E20" s="23">
         <f t="shared" si="5"/>
         <v>-3.0155349008501702</v>
       </c>
-      <c r="F20" s="34">
+      <c r="F20" s="28">
         <v>905</v>
       </c>
-      <c r="R20" s="31" t="s">
+      <c r="R20" s="25" t="s">
         <v>29</v>
       </c>
       <c r="S20" s="4">
@@ -17527,32 +17536,32 @@
       <c r="T20" s="4">
         <v>6.6880507097966502E-2</v>
       </c>
-      <c r="U20" s="22" t="s">
+      <c r="U20" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="V20" s="21"/>
+      <c r="V20" s="30"/>
     </row>
     <row r="21" spans="1:34" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A21" s="25"/>
-      <c r="B21" s="29">
+      <c r="A21" s="36"/>
+      <c r="B21" s="23">
         <v>0.52</v>
       </c>
-      <c r="C21" s="29">
-        <f>B21-'Carga e Descarga'!$G$17</f>
+      <c r="C21" s="23">
+        <f>B21-'Carga e Descarga'!$G$18</f>
         <v>0.10700000000000004</v>
       </c>
-      <c r="D21" s="29">
+      <c r="D21" s="23">
         <f t="shared" si="0"/>
         <v>0.25907990314769985</v>
       </c>
-      <c r="E21" s="29">
+      <c r="E21" s="23">
         <f t="shared" si="5"/>
         <v>-3.0155349008501702</v>
       </c>
-      <c r="F21" s="34">
+      <c r="F21" s="28">
         <v>944</v>
       </c>
-      <c r="R21" s="31" t="s">
+      <c r="R21" s="25" t="s">
         <v>43</v>
       </c>
       <c r="S21" s="4">
@@ -17561,20 +17570,20 @@
       <c r="T21" s="4">
         <v>0.13128518716578064</v>
       </c>
-      <c r="U21" s="22" t="s">
+      <c r="U21" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="V21" s="21"/>
+      <c r="V21" s="30"/>
     </row>
     <row r="23" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A23" s="23" t="s">
+      <c r="A23" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="B23" s="24"/>
-      <c r="C23" s="24"/>
-      <c r="D23" s="24"/>
-      <c r="E23" s="24"/>
-      <c r="F23" s="26"/>
+      <c r="B23" s="33"/>
+      <c r="C23" s="33"/>
+      <c r="D23" s="33"/>
+      <c r="E23" s="33"/>
+      <c r="F23" s="37"/>
     </row>
     <row r="24" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
@@ -17597,325 +17606,325 @@
       </c>
     </row>
     <row r="25" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A25" s="27">
+      <c r="A25" s="35">
         <v>1.0290000000000001E-2</v>
       </c>
-      <c r="B25" s="29">
+      <c r="B25" s="23">
         <v>0.41799999999999998</v>
       </c>
-      <c r="C25" s="29">
-        <f>B25-'Carga e Descarga'!$G$17</f>
+      <c r="C25" s="23">
+        <f>B25-'Carga e Descarga'!$G$18</f>
         <v>5.0000000000000044E-3</v>
       </c>
-      <c r="D25" s="29">
+      <c r="D25" s="23">
         <f t="shared" ref="D25:D39" si="8">C25/$P$18</f>
         <v>1.2106537530266356E-2</v>
       </c>
-      <c r="E25" s="29" t="s">
+      <c r="E25" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="F25" s="34">
+      <c r="F25" s="28">
         <v>12</v>
       </c>
     </row>
     <row r="26" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A26" s="25"/>
-      <c r="B26" s="29">
+      <c r="A26" s="36"/>
+      <c r="B26" s="23">
         <v>0.41699999999999998</v>
       </c>
-      <c r="C26" s="29">
-        <f>B26-'Carga e Descarga'!$G$17</f>
+      <c r="C26" s="23">
+        <f>B26-'Carga e Descarga'!$G$18</f>
         <v>4.0000000000000036E-3</v>
       </c>
-      <c r="D26" s="29">
+      <c r="D26" s="23">
         <f t="shared" si="8"/>
         <v>9.6852300242130842E-3</v>
       </c>
-      <c r="E26" s="29">
+      <c r="E26" s="23">
         <f>LN(C26)</f>
         <v>-5.5214609178622451</v>
       </c>
-      <c r="F26" s="34">
+      <c r="F26" s="28">
         <v>71</v>
       </c>
     </row>
     <row r="27" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A27" s="25"/>
-      <c r="B27" s="29">
+      <c r="A27" s="36"/>
+      <c r="B27" s="23">
         <v>0.41689999999999999</v>
       </c>
-      <c r="C27" s="29">
-        <f>B27-'Carga e Descarga'!$G$17</f>
+      <c r="C27" s="23">
+        <f>B27-'Carga e Descarga'!$G$18</f>
         <v>3.9000000000000146E-3</v>
       </c>
-      <c r="D27" s="29">
+      <c r="D27" s="23">
         <f t="shared" si="8"/>
         <v>9.4430992736077839E-3</v>
       </c>
-      <c r="E27" s="29">
+      <c r="E27" s="23">
         <f t="shared" ref="E27:E39" si="9">LN(C27)</f>
         <v>-5.5467787258465329</v>
       </c>
-      <c r="F27" s="34">
+      <c r="F27" s="28">
         <v>124</v>
       </c>
     </row>
     <row r="28" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A28" s="25"/>
-      <c r="B28" s="29">
+      <c r="A28" s="36"/>
+      <c r="B28" s="23">
         <v>0.41649999999999998</v>
       </c>
-      <c r="C28" s="29">
-        <f>B28-'Carga e Descarga'!$G$17</f>
+      <c r="C28" s="23">
+        <f>B28-'Carga e Descarga'!$G$18</f>
         <v>3.5000000000000031E-3</v>
       </c>
-      <c r="D28" s="29">
+      <c r="D28" s="23">
         <f t="shared" si="8"/>
         <v>8.4745762711864493E-3</v>
       </c>
-      <c r="E28" s="29">
+      <c r="E28" s="23">
         <f t="shared" si="9"/>
         <v>-5.6549923104867679</v>
       </c>
-      <c r="F28" s="34">
+      <c r="F28" s="28">
         <v>163</v>
       </c>
     </row>
     <row r="29" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A29" s="25"/>
-      <c r="B29" s="29">
+      <c r="A29" s="36"/>
+      <c r="B29" s="23">
         <v>0.41639999999999999</v>
       </c>
-      <c r="C29" s="29">
-        <f>B29-'Carga e Descarga'!$G$17</f>
+      <c r="C29" s="23">
+        <f>B29-'Carga e Descarga'!$G$18</f>
         <v>3.4000000000000141E-3</v>
       </c>
-      <c r="D29" s="29">
+      <c r="D29" s="23">
         <f t="shared" si="8"/>
         <v>8.2324455205811491E-3</v>
       </c>
-      <c r="E29" s="29">
+      <c r="E29" s="23">
         <f t="shared" si="9"/>
         <v>-5.6839798473600176</v>
       </c>
-      <c r="F29" s="34">
+      <c r="F29" s="28">
         <v>206</v>
       </c>
     </row>
     <row r="30" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A30" s="25"/>
-      <c r="B30" s="29">
+      <c r="A30" s="36"/>
+      <c r="B30" s="23">
         <v>0.4163</v>
       </c>
-      <c r="C30" s="29">
-        <f>B30-'Carga e Descarga'!$G$17</f>
+      <c r="C30" s="23">
+        <f>B30-'Carga e Descarga'!$G$18</f>
         <v>3.3000000000000251E-3</v>
       </c>
-      <c r="D30" s="29">
+      <c r="D30" s="23">
         <f t="shared" si="8"/>
         <v>7.9903147699758488E-3</v>
       </c>
-      <c r="E30" s="29">
+      <c r="E30" s="23">
         <f t="shared" si="9"/>
         <v>-5.7138328105096949</v>
       </c>
-      <c r="F30" s="34">
+      <c r="F30" s="28">
         <v>274</v>
       </c>
     </row>
     <row r="31" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A31" s="25"/>
-      <c r="B31" s="29">
+      <c r="A31" s="36"/>
+      <c r="B31" s="23">
         <v>0.41599999999999998</v>
       </c>
-      <c r="C31" s="29">
-        <f>B31-'Carga e Descarga'!$G$17</f>
+      <c r="C31" s="23">
+        <f>B31-'Carga e Descarga'!$G$18</f>
         <v>3.0000000000000027E-3</v>
       </c>
-      <c r="D31" s="29">
+      <c r="D31" s="23">
         <f t="shared" si="8"/>
         <v>7.2639225181598127E-3</v>
       </c>
-      <c r="E31" s="29">
+      <c r="E31" s="23">
         <f t="shared" si="9"/>
         <v>-5.8091429903140268</v>
       </c>
-      <c r="F31" s="34">
+      <c r="F31" s="28">
         <v>338</v>
       </c>
     </row>
     <row r="32" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A32" s="25"/>
-      <c r="B32" s="29">
+      <c r="A32" s="36"/>
+      <c r="B32" s="23">
         <v>0.41570000000000001</v>
       </c>
-      <c r="C32" s="29">
-        <f>B32-'Carga e Descarga'!$G$17</f>
+      <c r="C32" s="23">
+        <f>B32-'Carga e Descarga'!$G$18</f>
         <v>2.7000000000000357E-3</v>
       </c>
-      <c r="D32" s="29">
+      <c r="D32" s="23">
         <f t="shared" si="8"/>
         <v>6.5375302663439128E-3</v>
       </c>
-      <c r="E32" s="29">
+      <c r="E32" s="23">
         <f t="shared" si="9"/>
         <v>-5.9145035059718403</v>
       </c>
-      <c r="F32" s="34">
+      <c r="F32" s="28">
         <v>405</v>
       </c>
     </row>
     <row r="33" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A33" s="25"/>
-      <c r="B33" s="29">
+      <c r="A33" s="36"/>
+      <c r="B33" s="23">
         <v>0.41560000000000002</v>
       </c>
-      <c r="C33" s="29">
-        <f>B33-'Carga e Descarga'!$G$17</f>
+      <c r="C33" s="23">
+        <f>B33-'Carga e Descarga'!$G$18</f>
         <v>2.6000000000000467E-3</v>
       </c>
-      <c r="D33" s="29">
+      <c r="D33" s="23">
         <f t="shared" si="8"/>
         <v>6.2953995157386125E-3</v>
       </c>
-      <c r="E33" s="29">
+      <c r="E33" s="23">
         <f t="shared" si="9"/>
         <v>-5.9522438339546824</v>
       </c>
-      <c r="F33" s="34">
+      <c r="F33" s="28">
         <v>507</v>
       </c>
     </row>
     <row r="34" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A34" s="25"/>
-      <c r="B34" s="29">
+      <c r="A34" s="36"/>
+      <c r="B34" s="23">
         <v>0.41549999999999998</v>
       </c>
-      <c r="C34" s="29">
-        <f>B34-'Carga e Descarga'!$G$17</f>
+      <c r="C34" s="23">
+        <f>B34-'Carga e Descarga'!$G$18</f>
         <v>2.5000000000000022E-3</v>
       </c>
-      <c r="D34" s="29">
+      <c r="D34" s="23">
         <f t="shared" si="8"/>
         <v>6.0532687651331778E-3</v>
       </c>
-      <c r="E34" s="29">
+      <c r="E34" s="23">
         <f t="shared" si="9"/>
         <v>-5.9914645471079808</v>
       </c>
-      <c r="F34" s="34">
+      <c r="F34" s="28">
         <v>600</v>
       </c>
     </row>
     <row r="35" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A35" s="25"/>
-      <c r="B35" s="29">
+      <c r="A35" s="36"/>
+      <c r="B35" s="23">
         <v>0.41520000000000001</v>
       </c>
-      <c r="C35" s="29">
-        <f>B35-'Carga e Descarga'!$G$17</f>
+      <c r="C35" s="23">
+        <f>B35-'Carga e Descarga'!$G$18</f>
         <v>2.2000000000000353E-3</v>
       </c>
-      <c r="D35" s="29">
+      <c r="D35" s="23">
         <f t="shared" si="8"/>
         <v>5.3268765133172771E-3</v>
       </c>
-      <c r="E35" s="29">
+      <c r="E35" s="23">
         <f t="shared" si="9"/>
         <v>-6.1192979186178507</v>
       </c>
-      <c r="F35" s="34">
+      <c r="F35" s="28">
         <v>701</v>
       </c>
     </row>
     <row r="36" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A36" s="25"/>
-      <c r="B36" s="29">
+      <c r="A36" s="36"/>
+      <c r="B36" s="23">
         <v>0.41510000000000002</v>
       </c>
-      <c r="C36" s="29">
-        <f>B36-'Carga e Descarga'!$G$17</f>
+      <c r="C36" s="23">
+        <f>B36-'Carga e Descarga'!$G$18</f>
         <v>2.1000000000000463E-3</v>
       </c>
-      <c r="D36" s="29">
+      <c r="D36" s="23">
         <f t="shared" si="8"/>
         <v>5.0847457627119768E-3</v>
       </c>
-      <c r="E36" s="29">
+      <c r="E36" s="23">
         <f t="shared" si="9"/>
         <v>-6.1658179342527379</v>
       </c>
-      <c r="F36" s="34">
+      <c r="F36" s="28">
         <v>808</v>
       </c>
     </row>
     <row r="37" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A37" s="25"/>
-      <c r="B37" s="29">
+      <c r="A37" s="36"/>
+      <c r="B37" s="23">
         <v>0.41499999999999998</v>
       </c>
-      <c r="C37" s="29">
-        <f>B37-'Carga e Descarga'!$G$17</f>
+      <c r="C37" s="23">
+        <f>B37-'Carga e Descarga'!$G$18</f>
         <v>2.0000000000000018E-3</v>
       </c>
-      <c r="D37" s="29">
+      <c r="D37" s="23">
         <f t="shared" si="8"/>
         <v>4.8426150121065421E-3</v>
       </c>
-      <c r="E37" s="29">
+      <c r="E37" s="23">
         <f t="shared" si="9"/>
         <v>-6.2146080984221905</v>
       </c>
-      <c r="F37" s="34">
+      <c r="F37" s="28">
         <v>918</v>
       </c>
     </row>
     <row r="38" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A38" s="25"/>
-      <c r="B38" s="29">
+      <c r="A38" s="36"/>
+      <c r="B38" s="23">
         <v>0.41499999999999998</v>
       </c>
-      <c r="C38" s="29">
-        <f>B38-'Carga e Descarga'!$G$17</f>
+      <c r="C38" s="23">
+        <f>B38-'Carga e Descarga'!$G$18</f>
         <v>2.0000000000000018E-3</v>
       </c>
-      <c r="D38" s="29">
+      <c r="D38" s="23">
         <f t="shared" si="8"/>
         <v>4.8426150121065421E-3</v>
       </c>
-      <c r="E38" s="29">
+      <c r="E38" s="23">
         <f t="shared" si="9"/>
         <v>-6.2146080984221905</v>
       </c>
-      <c r="F38" s="34">
+      <c r="F38" s="28">
         <v>996</v>
       </c>
-      <c r="S38" s="21" t="s">
+      <c r="S38" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="T38" s="21"/>
+      <c r="T38" s="30"/>
     </row>
     <row r="39" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A39" s="25"/>
-      <c r="B39" s="29">
+      <c r="A39" s="36"/>
+      <c r="B39" s="23">
         <v>0.41499999999999998</v>
       </c>
-      <c r="C39" s="29">
-        <f>B39-'Carga e Descarga'!$G$17</f>
+      <c r="C39" s="23">
+        <f>B39-'Carga e Descarga'!$G$18</f>
         <v>2.0000000000000018E-3</v>
       </c>
-      <c r="D39" s="29">
+      <c r="D39" s="23">
         <f t="shared" si="8"/>
         <v>4.8426150121065421E-3</v>
       </c>
-      <c r="E39" s="29">
+      <c r="E39" s="23">
         <f t="shared" si="9"/>
         <v>-6.2146080984221905</v>
       </c>
-      <c r="F39" s="34">
+      <c r="F39" s="28">
         <v>1030</v>
       </c>
-      <c r="R39" s="31" t="s">
+      <c r="R39" s="25" t="s">
         <v>36</v>
       </c>
       <c r="S39" s="4">
@@ -17925,13 +17934,13 @@
       <c r="T39" s="4">
         <v>-5.5285241918709813</v>
       </c>
-      <c r="U39" s="22" t="s">
+      <c r="U39" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="V39" s="21"/>
+      <c r="V39" s="30"/>
     </row>
     <row r="40" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="R40" s="31" t="s">
+      <c r="R40" s="25" t="s">
         <v>29</v>
       </c>
       <c r="S40" s="4">
@@ -17940,13 +17949,13 @@
       <c r="T40" s="4">
         <v>2.7175572824945746E-2</v>
       </c>
-      <c r="U40" s="22" t="s">
+      <c r="U40" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="V40" s="21"/>
+      <c r="V40" s="30"/>
     </row>
     <row r="41" spans="1:22" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="R41" s="31" t="s">
+      <c r="R41" s="25" t="s">
         <v>43</v>
       </c>
       <c r="S41" s="4">
@@ -17955,10 +17964,10 @@
       <c r="T41" s="4">
         <v>5.4355580392070058E-2</v>
       </c>
-      <c r="U41" s="22" t="s">
+      <c r="U41" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="V41" s="21"/>
+      <c r="V41" s="30"/>
     </row>
     <row r="59" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D59" s="11"/>

</xml_diff>